<commit_message>
Refactor preset system: add Frequency/Chance presets, Damage Type Multipliers
- Remove IntensityPreset (redundant with DamagePreset)
- Remove GlobalDamageMultiplier
- Replace TickInterval slider with FrequencyPreset (Slow/Normal/Fast/Rapid)
- Add ChancePreset (Off/Rare/Default/Frequent/Always)
- Add per-zone Chance sliders
- Add Damage Type Multipliers section (Pierce/Slash/Blunt)
- Update BleedEffect to track DamageType for multiplier lookup
- Update BleedManager with chance roll logic
- Fix SyncOption to use correct ThunderRoad ModOption API
</commit_message>
<xml_diff>
--- a/MENU_MOCK.xlsx
+++ b/MENU_MOCK.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G44"/>
+  <dimension ref="A1:G46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -522,7 +522,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>OptionIntensityPreset</t>
+          <t>OptionDamagePreset</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -537,14 +537,10 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Overall bleed intensity. Applies multiplier values to all zones.</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>IntensityPresetProvider</t>
-        </is>
-      </c>
+          <t>Damage per tick preset. Applies damage values to all zones.</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -575,11 +571,7 @@
           <t>Bleed duration preset. Applies duration values to all zones.</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>DurationPresetProvider</t>
-        </is>
-      </c>
+      <c r="G4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -592,7 +584,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>OptionDamagePreset</t>
+          <t>OptionFrequencyPreset</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -602,19 +594,15 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>"Default"</t>
+          <t>"Normal"</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Damage per tick preset. Applies damage values to all zones.</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>DamagePresetProvider</t>
-        </is>
-      </c>
+          <t>Tick frequency preset. Controls how often damage ticks occur.</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -627,42 +615,38 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>OptionGlobalMultiplier</t>
+          <t>OptionChancePreset</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>float</t>
+          <t>string</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>1.0f</t>
+          <t>"Default"</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Final multiplier applied to all bleed damage</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>GlobalMultiplierProvider</t>
-        </is>
-      </c>
+          <t>Bleed chance preset. Applies chance values to all zones.</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>CategoryPresetSelection</t>
+          <t>CategoryDamageTypeMultipliers</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>OptionTickInterval</t>
+          <t>OptionPierceMultiplier</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -672,47 +656,43 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>0.5f</t>
+          <t>1.0f</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Time between damage ticks (all zones)</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>TickIntervalProvider</t>
-        </is>
-      </c>
+          <t>Damage multiplier for piercing attacks (stabs). Default 1.0x.</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>CategoryZoneToggles</t>
+          <t>CategoryDamageTypeMultipliers</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>OptionThroatEnabled</t>
+          <t>OptionSlashMultiplier</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>bool</t>
+          <t>float</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>true</t>
+          <t>1.0f</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Enable bleeding from throat wounds</t>
+          <t>Damage multiplier for slashing attacks (cuts). Default 1.0x.</t>
         </is>
       </c>
       <c r="G8" t="inlineStr"/>
@@ -720,30 +700,30 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>CategoryZoneToggles</t>
+          <t>CategoryDamageTypeMultipliers</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>OptionHeadEnabled</t>
+          <t>OptionBluntMultiplier</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>bool</t>
+          <t>float</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>true</t>
+          <t>1.0f</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Enable bleeding from head wounds</t>
+          <t>Damage multiplier for blunt attacks (impacts). Default 1.0x.</t>
         </is>
       </c>
       <c r="G9" t="inlineStr"/>
@@ -755,11 +735,11 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>OptionNeckEnabled</t>
+          <t>OptionThroatEnabled</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -774,7 +754,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Enable bleeding from neck wounds</t>
+          <t>Enable bleeding from throat wounds</t>
         </is>
       </c>
       <c r="G10" t="inlineStr"/>
@@ -786,11 +766,11 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>OptionTorsoEnabled</t>
+          <t>OptionHeadEnabled</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -805,7 +785,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Enable bleeding from torso wounds</t>
+          <t>Enable bleeding from head wounds</t>
         </is>
       </c>
       <c r="G11" t="inlineStr"/>
@@ -817,11 +797,11 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>OptionArmEnabled</t>
+          <t>OptionNeckEnabled</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -836,7 +816,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Enable bleeding from arm wounds</t>
+          <t>Enable bleeding from neck wounds</t>
         </is>
       </c>
       <c r="G12" t="inlineStr"/>
@@ -848,11 +828,11 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>OptionLegEnabled</t>
+          <t>OptionTorsoEnabled</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -867,7 +847,7 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Enable bleeding from leg wounds</t>
+          <t>Enable bleeding from torso wounds</t>
         </is>
       </c>
       <c r="G13" t="inlineStr"/>
@@ -879,11 +859,11 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>OptionDismembermentEnabled</t>
+          <t>OptionArmEnabled</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -898,7 +878,7 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Enable bleeding from dismemberment</t>
+          <t>Enable bleeding from arm wounds</t>
         </is>
       </c>
       <c r="G14" t="inlineStr"/>
@@ -906,72 +886,64 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>CategoryZoneThroat</t>
+          <t>CategoryZoneToggles</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>OptionThroatMultiplier</t>
+          <t>OptionLegEnabled</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>float</t>
+          <t>bool</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>3.0f</t>
+          <t>true</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Damage multiplier for throat wounds</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>MultiplierProvider</t>
-        </is>
-      </c>
+          <t>Enable bleeding from leg wounds</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>CategoryZoneThroat</t>
+          <t>CategoryZoneToggles</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>20</v>
+        <v>70</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>OptionThroatDuration</t>
+          <t>OptionDismembermentEnabled</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>float</t>
+          <t>bool</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>8.0f</t>
+          <t>true</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>How long throat bleeds last</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>DurationProvider</t>
-        </is>
-      </c>
+          <t>Enable bleeding from dismemberment</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -980,11 +952,11 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>OptionThroatDamagePerTick</t>
+          <t>OptionThroatChance</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -994,19 +966,15 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>5.0f</t>
+          <t>75f</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Base damage per tick for throat wounds</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>DamagePerTickProvider</t>
-        </is>
-      </c>
+          <t>Chance for throat wounds to cause bleeding</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1015,46 +983,42 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>OptionThroatStackLimit</t>
+          <t>OptionThroatDamage</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>int</t>
+          <t>float</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>5.0f</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Max stacks for throat wounds</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>StackLimitProvider</t>
-        </is>
-      </c>
+          <t>Base damage per tick for throat wounds</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>CategoryZoneHead</t>
+          <t>CategoryZoneThroat</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>OptionHeadMultiplier</t>
+          <t>OptionThroatDuration</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -1064,54 +1028,46 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>2.0f</t>
+          <t>8.0f</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Damage multiplier for head wounds</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>MultiplierProvider</t>
-        </is>
-      </c>
+          <t>How long throat bleeds last</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>CategoryZoneHead</t>
+          <t>CategoryZoneThroat</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>OptionHeadDuration</t>
+          <t>OptionThroatStackLimit</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>float</t>
+          <t>int</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>6.0f</t>
+          <t>3</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>How long head bleeds last</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>DurationProvider</t>
-        </is>
-      </c>
+          <t>Max stacks for throat wounds</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1120,11 +1076,11 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>OptionHeadDamagePerTick</t>
+          <t>OptionHeadChance</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1134,19 +1090,15 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>3.0f</t>
+          <t>50f</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Base damage per tick for head wounds</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>DamagePerTickProvider</t>
-        </is>
-      </c>
+          <t>Chance for head wounds to cause bleeding</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1155,46 +1107,42 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>OptionHeadStackLimit</t>
+          <t>OptionHeadDamage</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>int</t>
+          <t>float</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>3.0f</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Max stacks for head wounds</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>StackLimitProvider</t>
-        </is>
-      </c>
+          <t>Base damage per tick for head wounds</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>CategoryZoneNeck</t>
+          <t>CategoryZoneHead</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>OptionNeckMultiplier</t>
+          <t>OptionHeadDuration</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -1204,54 +1152,46 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>2.5f</t>
+          <t>6.0f</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Damage multiplier for neck wounds</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>MultiplierProvider</t>
-        </is>
-      </c>
+          <t>How long head bleeds last</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>CategoryZoneNeck</t>
+          <t>CategoryZoneHead</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>OptionNeckDuration</t>
+          <t>OptionHeadStackLimit</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>float</t>
+          <t>int</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>7.0f</t>
+          <t>3</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>How long neck bleeds last</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>DurationProvider</t>
-        </is>
-      </c>
+          <t>Max stacks for head wounds</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1260,11 +1200,11 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>OptionNeckDamagePerTick</t>
+          <t>OptionNeckChance</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1274,19 +1214,15 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>4.0f</t>
+          <t>65f</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Base damage per tick for neck wounds</t>
-        </is>
-      </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>DamagePerTickProvider</t>
-        </is>
-      </c>
+          <t>Chance for neck wounds to cause bleeding</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1295,46 +1231,42 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>OptionNeckStackLimit</t>
+          <t>OptionNeckDamage</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>int</t>
+          <t>float</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4.0f</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Max stacks for neck wounds</t>
-        </is>
-      </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>StackLimitProvider</t>
-        </is>
-      </c>
+          <t>Base damage per tick for neck wounds</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>CategoryZoneTorso</t>
+          <t>CategoryZoneNeck</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>OptionTorsoMultiplier</t>
+          <t>OptionNeckDuration</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1344,54 +1276,46 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>1.0f</t>
+          <t>7.0f</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Damage multiplier for torso wounds</t>
-        </is>
-      </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>MultiplierProvider</t>
-        </is>
-      </c>
+          <t>How long neck bleeds last</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>CategoryZoneTorso</t>
+          <t>CategoryZoneNeck</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>OptionTorsoDuration</t>
+          <t>OptionNeckStackLimit</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>float</t>
+          <t>int</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>5.0f</t>
+          <t>3</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>How long torso bleeds last</t>
-        </is>
-      </c>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t>DurationProvider</t>
-        </is>
-      </c>
+          <t>Max stacks for neck wounds</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1400,11 +1324,11 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>OptionTorsoDamagePerTick</t>
+          <t>OptionTorsoChance</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -1414,19 +1338,15 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>2.0f</t>
+          <t>40f</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Base damage per tick for torso wounds</t>
-        </is>
-      </c>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t>DamagePerTickProvider</t>
-        </is>
-      </c>
+          <t>Chance for torso wounds to cause bleeding</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1435,46 +1355,42 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>OptionTorsoStackLimit</t>
+          <t>OptionTorsoDamage</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>int</t>
+          <t>float</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>2.0f</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Max stacks for torso wounds</t>
-        </is>
-      </c>
-      <c r="G30" t="inlineStr">
-        <is>
-          <t>StackLimitProvider</t>
-        </is>
-      </c>
+          <t>Base damage per tick for torso wounds</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>CategoryZoneArm</t>
+          <t>CategoryZoneTorso</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>OptionArmMultiplier</t>
+          <t>OptionTorsoDuration</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1484,54 +1400,46 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>0.5f</t>
+          <t>5.0f</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>Damage multiplier for arm wounds</t>
-        </is>
-      </c>
-      <c r="G31" t="inlineStr">
-        <is>
-          <t>MultiplierProvider</t>
-        </is>
-      </c>
+          <t>How long torso bleeds last</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>CategoryZoneArm</t>
+          <t>CategoryZoneTorso</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>OptionArmDuration</t>
+          <t>OptionTorsoStackLimit</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>float</t>
+          <t>int</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>4.0f</t>
+          <t>5</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>How long arm bleeds last</t>
-        </is>
-      </c>
-      <c r="G32" t="inlineStr">
-        <is>
-          <t>DurationProvider</t>
-        </is>
-      </c>
+          <t>Max stacks for torso wounds</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1540,11 +1448,11 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>OptionArmDamagePerTick</t>
+          <t>OptionArmChance</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -1554,19 +1462,15 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>1.0f</t>
+          <t>30f</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>Base damage per tick for arm wounds</t>
-        </is>
-      </c>
-      <c r="G33" t="inlineStr">
-        <is>
-          <t>DamagePerTickProvider</t>
-        </is>
-      </c>
+          <t>Chance for arm wounds to cause bleeding</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1575,46 +1479,42 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>OptionArmStackLimit</t>
+          <t>OptionArmDamage</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>int</t>
+          <t>float</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1.0f</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Max stacks for arm wounds</t>
-        </is>
-      </c>
-      <c r="G34" t="inlineStr">
-        <is>
-          <t>StackLimitProvider</t>
-        </is>
-      </c>
+          <t>Base damage per tick for arm wounds</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>CategoryZoneLeg</t>
+          <t>CategoryZoneArm</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>OptionLegMultiplier</t>
+          <t>OptionArmDuration</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -1624,54 +1524,46 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>0.6f</t>
+          <t>4.0f</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>Damage multiplier for leg wounds</t>
-        </is>
-      </c>
-      <c r="G35" t="inlineStr">
-        <is>
-          <t>MultiplierProvider</t>
-        </is>
-      </c>
+          <t>How long arm bleeds last</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>CategoryZoneLeg</t>
+          <t>CategoryZoneArm</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>OptionLegDuration</t>
+          <t>OptionArmStackLimit</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>float</t>
+          <t>int</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>5.0f</t>
+          <t>4</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>How long leg bleeds last</t>
-        </is>
-      </c>
-      <c r="G36" t="inlineStr">
-        <is>
-          <t>DurationProvider</t>
-        </is>
-      </c>
+          <t>Max stacks for arm wounds</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1680,11 +1572,11 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>OptionLegDamagePerTick</t>
+          <t>OptionLegChance</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -1694,19 +1586,15 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>1.5f</t>
+          <t>35f</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>Base damage per tick for leg wounds</t>
-        </is>
-      </c>
-      <c r="G37" t="inlineStr">
-        <is>
-          <t>DamagePerTickProvider</t>
-        </is>
-      </c>
+          <t>Chance for leg wounds to cause bleeding</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1715,46 +1603,42 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>OptionLegStackLimit</t>
+          <t>OptionLegDamage</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>int</t>
+          <t>float</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1.5f</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>Max stacks for leg wounds</t>
-        </is>
-      </c>
-      <c r="G38" t="inlineStr">
-        <is>
-          <t>StackLimitProvider</t>
-        </is>
-      </c>
+          <t>Base damage per tick for leg wounds</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>CategoryZoneDismemberment</t>
+          <t>CategoryZoneLeg</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>OptionDismembermentMultiplier</t>
+          <t>OptionLegDuration</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -1764,54 +1648,46 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>2.5f</t>
+          <t>5.0f</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>Damage multiplier for dismemberment</t>
-        </is>
-      </c>
-      <c r="G39" t="inlineStr">
-        <is>
-          <t>MultiplierProvider</t>
-        </is>
-      </c>
+          <t>How long leg bleeds last</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>CategoryZoneDismemberment</t>
+          <t>CategoryZoneLeg</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>OptionDismembermentDuration</t>
+          <t>OptionLegStackLimit</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>float</t>
+          <t>int</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>10.0f</t>
+          <t>4</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>How long dismemberment bleeds last</t>
-        </is>
-      </c>
-      <c r="G40" t="inlineStr">
-        <is>
-          <t>DurationProvider</t>
-        </is>
-      </c>
+          <t>Max stacks for leg wounds</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1820,11 +1696,11 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>OptionDismembermentDamagePerTick</t>
+          <t>OptionDismembermentChance</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -1834,19 +1710,15 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>6.0f</t>
+          <t>100f</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>Base damage per tick for dismemberment</t>
-        </is>
-      </c>
-      <c r="G41" t="inlineStr">
-        <is>
-          <t>DamagePerTickProvider</t>
-        </is>
-      </c>
+          <t>Chance for dismemberment to cause bleeding</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -1855,61 +1727,57 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>OptionDismembermentStackLimit</t>
+          <t>OptionDismembermentDamage</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>int</t>
+          <t>float</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>6.0f</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>Max stacks for dismemberment (per limb)</t>
-        </is>
-      </c>
-      <c r="G42" t="inlineStr">
-        <is>
-          <t>StackLimitProvider</t>
-        </is>
-      </c>
+          <t>Base damage per tick for dismemberment</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>CategoryAdvanced</t>
+          <t>CategoryZoneDismemberment</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>OptionDebugLogging</t>
+          <t>OptionDismembermentDuration</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>bool</t>
+          <t>float</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>false</t>
+          <t>10.0f</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>Enable verbose debug logging</t>
+          <t>How long dismemberment bleeds last</t>
         </is>
       </c>
       <c r="G43" t="inlineStr"/>
@@ -1917,33 +1785,95 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
+          <t>CategoryZoneDismemberment</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>40</v>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>OptionDismembermentStackLimit</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>int</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>Max stacks for dismemberment (per limb)</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr"/>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>CategoryAdvanced</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>10</v>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>OptionDebugLogging</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>bool</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>Enable verbose debug logging</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr"/>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
           <t>CategoryStatistics</t>
         </is>
       </c>
-      <c r="B44" t="n">
+      <c r="B46" t="n">
         <v>10</v>
       </c>
-      <c r="C44" t="inlineStr">
+      <c r="C46" t="inlineStr">
         <is>
           <t>OptionResetStats</t>
         </is>
       </c>
-      <c r="D44" t="inlineStr">
+      <c r="D46" t="inlineStr">
         <is>
           <t>bool</t>
         </is>
       </c>
-      <c r="E44" t="inlineStr">
+      <c r="E46" t="inlineStr">
         <is>
           <t>false</t>
         </is>
       </c>
-      <c r="F44" t="inlineStr">
+      <c r="F46" t="inlineStr">
         <is>
           <t>Toggle to reset all statistics</t>
         </is>
       </c>
-      <c r="G44" t="inlineStr"/>
+      <c r="G46" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
5-preset system with lower defaults, multiplier fix, xlsx generators
</commit_message>
<xml_diff>
--- a/MENU_MOCK.xlsx
+++ b/MENU_MOCK.xlsx
@@ -537,7 +537,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Damage per tick preset. Applies damage values to all zones.</t>
+          <t>Damage per tick preset. Default is the balanced middle value.</t>
         </is>
       </c>
       <c r="G3" t="inlineStr"/>
@@ -568,7 +568,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Bleed duration preset. Applies duration values to all zones.</t>
+          <t>Bleed duration preset. Default is the balanced middle value.</t>
         </is>
       </c>
       <c r="G4" t="inlineStr"/>
@@ -594,12 +594,12 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>"Normal"</t>
+          <t>"Default"</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Tick frequency preset. Controls how often damage ticks occur.</t>
+          <t>Tick frequency preset. Default is the balanced middle value.</t>
         </is>
       </c>
       <c r="G5" t="inlineStr"/>
@@ -630,7 +630,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Bleed chance preset. Applies chance values to all zones.</t>
+          <t>Bleed chance preset. Default is the balanced middle value.</t>
         </is>
       </c>
       <c r="G6" t="inlineStr"/>
@@ -661,7 +661,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Damage multiplier for piercing attacks (stabs). Default 1.0x.</t>
+          <t>Bleed damage multiplier for pierce attacks. 0.0x disables bleed from pierce entirely.</t>
         </is>
       </c>
       <c r="G7" t="inlineStr"/>
@@ -692,7 +692,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Damage multiplier for slashing attacks (cuts). Default 1.0x.</t>
+          <t>Bleed damage multiplier for slash attacks. 0.0x disables bleed from slash entirely.</t>
         </is>
       </c>
       <c r="G8" t="inlineStr"/>
@@ -718,12 +718,12 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>1.0f</t>
+          <t>0.5f</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Damage multiplier for blunt attacks (impacts). Default 1.0x.</t>
+          <t>Bleed damage multiplier for blunt attacks. 0.0x disables bleed from blunt entirely.</t>
         </is>
       </c>
       <c r="G9" t="inlineStr"/>
@@ -966,7 +966,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>75f</t>
+          <t>60f</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -997,7 +997,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>5.0f</t>
+          <t>2.5f</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1028,7 +1028,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>8.0f</t>
+          <t>6.0f</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1090,7 +1090,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>50f</t>
+          <t>40f</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1121,7 +1121,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>3.0f</t>
+          <t>1.5f</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -1152,7 +1152,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>6.0f</t>
+          <t>5.0f</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -1214,7 +1214,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>65f</t>
+          <t>55f</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -1245,7 +1245,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>4.0f</t>
+          <t>2.0f</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -1276,7 +1276,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>7.0f</t>
+          <t>5.5f</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -1338,7 +1338,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>40f</t>
+          <t>35f</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -1369,7 +1369,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>2.0f</t>
+          <t>1.0f</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -1400,7 +1400,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>5.0f</t>
+          <t>4.0f</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -1462,7 +1462,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>30f</t>
+          <t>25f</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -1493,7 +1493,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>1.0f</t>
+          <t>0.5f</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -1524,7 +1524,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>4.0f</t>
+          <t>3.0f</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -1586,7 +1586,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>35f</t>
+          <t>30f</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -1617,7 +1617,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>1.5f</t>
+          <t>0.75f</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -1648,7 +1648,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>5.0f</t>
+          <t>3.5f</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -1710,7 +1710,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>100f</t>
+          <t>80f</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -1741,7 +1741,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>6.0f</t>
+          <t>3.0f</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -1772,7 +1772,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>10.0f</t>
+          <t>8.0f</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">

</xml_diff>

<commit_message>
Per-zone frequency, slider range 0.1-5.0s, AI disclaimer in PUBLISH.md
</commit_message>
<xml_diff>
--- a/MENU_MOCK.xlsx
+++ b/MENU_MOCK.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G46"/>
+  <dimension ref="A1:G53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1045,26 +1045,26 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>OptionThroatStackLimit</t>
+          <t>OptionThroatFrequency</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>int</t>
+          <t>float</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>0.5f</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Max stacks for throat wounds</t>
+          <t>Time between bleed ticks for throat wounds</t>
         </is>
       </c>
       <c r="G20" t="inlineStr"/>
@@ -1072,30 +1072,30 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>CategoryZoneHead</t>
+          <t>CategoryZoneThroat</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>OptionHeadChance</t>
+          <t>OptionThroatStackLimit</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>float</t>
+          <t>int</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>40f</t>
+          <t>3</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Chance for head wounds to cause bleeding</t>
+          <t>Max stacks for throat wounds</t>
         </is>
       </c>
       <c r="G21" t="inlineStr"/>
@@ -1107,11 +1107,11 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>OptionHeadDamage</t>
+          <t>OptionHeadChance</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -1121,12 +1121,12 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>1.5f</t>
+          <t>40f</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Base damage per tick for head wounds</t>
+          <t>Chance for head wounds to cause bleeding</t>
         </is>
       </c>
       <c r="G22" t="inlineStr"/>
@@ -1138,11 +1138,11 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>OptionHeadDuration</t>
+          <t>OptionHeadDamage</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -1152,12 +1152,12 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>5.0f</t>
+          <t>1.5f</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>How long head bleeds last</t>
+          <t>Base damage per tick for head wounds</t>
         </is>
       </c>
       <c r="G23" t="inlineStr"/>
@@ -1169,26 +1169,26 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>OptionHeadStackLimit</t>
+          <t>OptionHeadDuration</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>int</t>
+          <t>float</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>5.0f</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Max stacks for head wounds</t>
+          <t>How long head bleeds last</t>
         </is>
       </c>
       <c r="G24" t="inlineStr"/>
@@ -1196,15 +1196,15 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>CategoryZoneNeck</t>
+          <t>CategoryZoneHead</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>OptionNeckChance</t>
+          <t>OptionHeadFrequency</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1214,12 +1214,12 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>55f</t>
+          <t>0.5f</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Chance for neck wounds to cause bleeding</t>
+          <t>Time between bleed ticks for head wounds</t>
         </is>
       </c>
       <c r="G25" t="inlineStr"/>
@@ -1227,30 +1227,30 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>CategoryZoneNeck</t>
+          <t>CategoryZoneHead</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>OptionNeckDamage</t>
+          <t>OptionHeadStackLimit</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>float</t>
+          <t>int</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>2.0f</t>
+          <t>3</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Base damage per tick for neck wounds</t>
+          <t>Max stacks for head wounds</t>
         </is>
       </c>
       <c r="G26" t="inlineStr"/>
@@ -1262,11 +1262,11 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>OptionNeckDuration</t>
+          <t>OptionNeckChance</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1276,12 +1276,12 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>5.5f</t>
+          <t>55f</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>How long neck bleeds last</t>
+          <t>Chance for neck wounds to cause bleeding</t>
         </is>
       </c>
       <c r="G27" t="inlineStr"/>
@@ -1293,26 +1293,26 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>OptionNeckStackLimit</t>
+          <t>OptionNeckDamage</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>int</t>
+          <t>float</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2.0f</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>Max stacks for neck wounds</t>
+          <t>Base damage per tick for neck wounds</t>
         </is>
       </c>
       <c r="G28" t="inlineStr"/>
@@ -1320,15 +1320,15 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>CategoryZoneTorso</t>
+          <t>CategoryZoneNeck</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>OptionTorsoChance</t>
+          <t>OptionNeckDuration</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -1338,12 +1338,12 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>35f</t>
+          <t>5.5f</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Chance for torso wounds to cause bleeding</t>
+          <t>How long neck bleeds last</t>
         </is>
       </c>
       <c r="G29" t="inlineStr"/>
@@ -1351,15 +1351,15 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>CategoryZoneTorso</t>
+          <t>CategoryZoneNeck</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>OptionTorsoDamage</t>
+          <t>OptionNeckFrequency</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -1369,12 +1369,12 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>1.0f</t>
+          <t>0.5f</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Base damage per tick for torso wounds</t>
+          <t>Time between bleed ticks for neck wounds</t>
         </is>
       </c>
       <c r="G30" t="inlineStr"/>
@@ -1382,30 +1382,30 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>CategoryZoneTorso</t>
+          <t>CategoryZoneNeck</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>OptionTorsoDuration</t>
+          <t>OptionNeckStackLimit</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>float</t>
+          <t>int</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>4.0f</t>
+          <t>3</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>How long torso bleeds last</t>
+          <t>Max stacks for neck wounds</t>
         </is>
       </c>
       <c r="G31" t="inlineStr"/>
@@ -1417,26 +1417,26 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>OptionTorsoStackLimit</t>
+          <t>OptionTorsoChance</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>int</t>
+          <t>float</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>35f</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>Max stacks for torso wounds</t>
+          <t>Chance for torso wounds to cause bleeding</t>
         </is>
       </c>
       <c r="G32" t="inlineStr"/>
@@ -1444,15 +1444,15 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>CategoryZoneArm</t>
+          <t>CategoryZoneTorso</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>OptionArmChance</t>
+          <t>OptionTorsoDamage</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -1462,12 +1462,12 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>25f</t>
+          <t>1.0f</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>Chance for arm wounds to cause bleeding</t>
+          <t>Base damage per tick for torso wounds</t>
         </is>
       </c>
       <c r="G33" t="inlineStr"/>
@@ -1475,15 +1475,15 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>CategoryZoneArm</t>
+          <t>CategoryZoneTorso</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>OptionArmDamage</t>
+          <t>OptionTorsoDuration</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -1493,12 +1493,12 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>0.5f</t>
+          <t>4.0f</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Base damage per tick for arm wounds</t>
+          <t>How long torso bleeds last</t>
         </is>
       </c>
       <c r="G34" t="inlineStr"/>
@@ -1506,15 +1506,15 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>CategoryZoneArm</t>
+          <t>CategoryZoneTorso</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>OptionArmDuration</t>
+          <t>OptionTorsoFrequency</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -1524,12 +1524,12 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>3.0f</t>
+          <t>0.5f</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>How long arm bleeds last</t>
+          <t>Time between bleed ticks for torso wounds</t>
         </is>
       </c>
       <c r="G35" t="inlineStr"/>
@@ -1537,7 +1537,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>CategoryZoneArm</t>
+          <t>CategoryZoneTorso</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -1545,7 +1545,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>OptionArmStackLimit</t>
+          <t>OptionTorsoStackLimit</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -1555,12 +1555,12 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>Max stacks for arm wounds</t>
+          <t>Max stacks for torso wounds</t>
         </is>
       </c>
       <c r="G36" t="inlineStr"/>
@@ -1568,7 +1568,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>CategoryZoneLeg</t>
+          <t>CategoryZoneArm</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -1576,7 +1576,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>OptionLegChance</t>
+          <t>OptionArmChance</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -1586,12 +1586,12 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>30f</t>
+          <t>25f</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>Chance for leg wounds to cause bleeding</t>
+          <t>Chance for arm wounds to cause bleeding</t>
         </is>
       </c>
       <c r="G37" t="inlineStr"/>
@@ -1599,7 +1599,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>CategoryZoneLeg</t>
+          <t>CategoryZoneArm</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -1607,7 +1607,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>OptionLegDamage</t>
+          <t>OptionArmDamage</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -1617,12 +1617,12 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>0.75f</t>
+          <t>0.5f</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>Base damage per tick for leg wounds</t>
+          <t>Base damage per tick for arm wounds</t>
         </is>
       </c>
       <c r="G38" t="inlineStr"/>
@@ -1630,7 +1630,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>CategoryZoneLeg</t>
+          <t>CategoryZoneArm</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -1638,7 +1638,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>OptionLegDuration</t>
+          <t>OptionArmDuration</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -1648,12 +1648,12 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>3.5f</t>
+          <t>3.0f</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>How long leg bleeds last</t>
+          <t>How long arm bleeds last</t>
         </is>
       </c>
       <c r="G39" t="inlineStr"/>
@@ -1661,30 +1661,30 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>CategoryZoneLeg</t>
+          <t>CategoryZoneArm</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>OptionLegStackLimit</t>
+          <t>OptionArmFrequency</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>int</t>
+          <t>float</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>0.5f</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>Max stacks for leg wounds</t>
+          <t>Time between bleed ticks for arm wounds</t>
         </is>
       </c>
       <c r="G40" t="inlineStr"/>
@@ -1692,30 +1692,30 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>CategoryZoneDismemberment</t>
+          <t>CategoryZoneArm</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>OptionDismembermentChance</t>
+          <t>OptionArmStackLimit</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>float</t>
+          <t>int</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>80f</t>
+          <t>4</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>Chance for dismemberment to cause bleeding</t>
+          <t>Max stacks for arm wounds</t>
         </is>
       </c>
       <c r="G41" t="inlineStr"/>
@@ -1723,15 +1723,15 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>CategoryZoneDismemberment</t>
+          <t>CategoryZoneLeg</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>OptionDismembermentDamage</t>
+          <t>OptionLegChance</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -1741,12 +1741,12 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>3.0f</t>
+          <t>30f</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>Base damage per tick for dismemberment</t>
+          <t>Chance for leg wounds to cause bleeding</t>
         </is>
       </c>
       <c r="G42" t="inlineStr"/>
@@ -1754,15 +1754,15 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>CategoryZoneDismemberment</t>
+          <t>CategoryZoneLeg</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>OptionDismembermentDuration</t>
+          <t>OptionLegDamage</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -1772,12 +1772,12 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>8.0f</t>
+          <t>0.75f</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>How long dismemberment bleeds last</t>
+          <t>Base damage per tick for leg wounds</t>
         </is>
       </c>
       <c r="G43" t="inlineStr"/>
@@ -1785,30 +1785,30 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>CategoryZoneDismemberment</t>
+          <t>CategoryZoneLeg</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>OptionDismembermentStackLimit</t>
+          <t>OptionLegDuration</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>int</t>
+          <t>float</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3.5f</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>Max stacks for dismemberment (per limb)</t>
+          <t>How long leg bleeds last</t>
         </is>
       </c>
       <c r="G44" t="inlineStr"/>
@@ -1816,30 +1816,30 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>CategoryAdvanced</t>
+          <t>CategoryZoneLeg</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>OptionDebugLogging</t>
+          <t>OptionLegFrequency</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>bool</t>
+          <t>float</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>false</t>
+          <t>0.5f</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>Enable verbose debug logging</t>
+          <t>Time between bleed ticks for leg wounds</t>
         </is>
       </c>
       <c r="G45" t="inlineStr"/>
@@ -1847,33 +1847,250 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
+          <t>CategoryZoneLeg</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>40</v>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>OptionLegStackLimit</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>int</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>Max stacks for leg wounds</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr"/>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>CategoryZoneDismemberment</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>10</v>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>OptionDismembermentChance</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>float</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>80f</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>Chance for dismemberment to cause bleeding</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr"/>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>CategoryZoneDismemberment</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>20</v>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>OptionDismembermentDamage</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>float</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>3.0f</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>Base damage per tick for dismemberment</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr"/>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>CategoryZoneDismemberment</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>30</v>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>OptionDismembermentDuration</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>float</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>8.0f</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>How long dismemberment bleeds last</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr"/>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>CategoryZoneDismemberment</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>35</v>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>OptionDismembermentFrequency</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>float</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>0.5f</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>Time between bleed ticks for dismemberment</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr"/>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>CategoryZoneDismemberment</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>40</v>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>OptionDismembermentStackLimit</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>int</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>Max stacks for dismemberment (per limb)</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr"/>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>CategoryAdvanced</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>10</v>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>OptionDebugLogging</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>bool</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>Enable verbose debug logging</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr"/>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
           <t>CategoryStatistics</t>
         </is>
       </c>
-      <c r="B46" t="n">
+      <c r="B53" t="n">
         <v>10</v>
       </c>
-      <c r="C46" t="inlineStr">
+      <c r="C53" t="inlineStr">
         <is>
           <t>OptionResetStats</t>
         </is>
       </c>
-      <c r="D46" t="inlineStr">
+      <c r="D53" t="inlineStr">
         <is>
           <t>bool</t>
         </is>
       </c>
-      <c r="E46" t="inlineStr">
+      <c r="E53" t="inlineStr">
         <is>
           <t>false</t>
         </is>
       </c>
-      <c r="F46" t="inlineStr">
+      <c r="F53" t="inlineStr">
         <is>
           <t>Toggle to reset all statistics</t>
         </is>
       </c>
-      <c r="G46" t="inlineStr"/>
+      <c r="G53" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Add Profile preset (Default/BleedOnly/ElementalOnly), elemental damage type multipliers
</commit_message>
<xml_diff>
--- a/MENU_MOCK.xlsx
+++ b/MENU_MOCK.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G53"/>
+  <dimension ref="A1:G57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -518,11 +518,11 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>OptionDamagePreset</t>
+          <t>OptionProfilePreset</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -537,7 +537,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Damage per tick preset. Default is the balanced middle value.</t>
+          <t>Profile determines which damage types trigger DOT effects. Default/BleedOnly = physical attacks, ElementalOnly = fire/lightning/energy attacks.</t>
         </is>
       </c>
       <c r="G3" t="inlineStr"/>
@@ -549,11 +549,11 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>OptionDurationPreset</t>
+          <t>OptionDamagePreset</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -568,7 +568,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Bleed duration preset. Default is the balanced middle value.</t>
+          <t>Damage per tick preset. Default is the balanced middle value.</t>
         </is>
       </c>
       <c r="G4" t="inlineStr"/>
@@ -580,11 +580,11 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>OptionFrequencyPreset</t>
+          <t>OptionDurationPreset</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -599,7 +599,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Tick frequency preset. Default is the balanced middle value.</t>
+          <t>Bleed duration preset. Default is the balanced middle value.</t>
         </is>
       </c>
       <c r="G5" t="inlineStr"/>
@@ -611,11 +611,11 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>OptionChancePreset</t>
+          <t>OptionFrequencyPreset</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -630,7 +630,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Bleed chance preset. Default is the balanced middle value.</t>
+          <t>Tick frequency preset. Default is the balanced middle value.</t>
         </is>
       </c>
       <c r="G6" t="inlineStr"/>
@@ -638,30 +638,30 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>CategoryDamageTypeMultipliers</t>
+          <t>CategoryPresetSelection</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>OptionPierceMultiplier</t>
+          <t>OptionChancePreset</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>float</t>
+          <t>string</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>1.0f</t>
+          <t>"Default"</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Bleed damage multiplier for pierce attacks. 0.0x disables bleed from pierce entirely.</t>
+          <t>Bleed chance preset. Default is the balanced middle value.</t>
         </is>
       </c>
       <c r="G7" t="inlineStr"/>
@@ -673,11 +673,11 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>OptionSlashMultiplier</t>
+          <t>OptionPierceMultiplier</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -692,7 +692,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Bleed damage multiplier for slash attacks. 0.0x disables bleed from slash entirely.</t>
+          <t>DOT damage multiplier for pierce attacks. 0.0x disables DOT from pierce entirely.</t>
         </is>
       </c>
       <c r="G8" t="inlineStr"/>
@@ -704,11 +704,11 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>OptionBluntMultiplier</t>
+          <t>OptionSlashMultiplier</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -718,12 +718,12 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>0.5f</t>
+          <t>1.0f</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Bleed damage multiplier for blunt attacks. 0.0x disables bleed from blunt entirely.</t>
+          <t>DOT damage multiplier for slash attacks. 0.0x disables DOT from slash entirely.</t>
         </is>
       </c>
       <c r="G9" t="inlineStr"/>
@@ -731,30 +731,30 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>CategoryZoneToggles</t>
+          <t>CategoryDamageTypeMultipliers</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>OptionThroatEnabled</t>
+          <t>OptionBluntMultiplier</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>bool</t>
+          <t>float</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>true</t>
+          <t>0.5f</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Enable bleeding from throat wounds</t>
+          <t>DOT damage multiplier for blunt attacks. 0.0x disables DOT from blunt entirely.</t>
         </is>
       </c>
       <c r="G10" t="inlineStr"/>
@@ -762,30 +762,30 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>CategoryZoneToggles</t>
+          <t>CategoryDamageTypeMultipliers</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>OptionHeadEnabled</t>
+          <t>OptionFireMultiplier</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>bool</t>
+          <t>float</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>true</t>
+          <t>1.0f</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Enable bleeding from head wounds</t>
+          <t>DOT damage multiplier for fire attacks. 0.0x disables DOT from fire entirely.</t>
         </is>
       </c>
       <c r="G11" t="inlineStr"/>
@@ -793,30 +793,30 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>CategoryZoneToggles</t>
+          <t>CategoryDamageTypeMultipliers</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>OptionNeckEnabled</t>
+          <t>OptionLightningMultiplier</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>bool</t>
+          <t>float</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>true</t>
+          <t>1.0f</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Enable bleeding from neck wounds</t>
+          <t>DOT damage multiplier for lightning attacks. 0.0x disables DOT from lightning entirely.</t>
         </is>
       </c>
       <c r="G12" t="inlineStr"/>
@@ -824,30 +824,30 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>CategoryZoneToggles</t>
+          <t>CategoryDamageTypeMultipliers</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>OptionTorsoEnabled</t>
+          <t>OptionEnergyMultiplier</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>bool</t>
+          <t>float</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>true</t>
+          <t>1.0f</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Enable bleeding from torso wounds</t>
+          <t>DOT damage multiplier for energy attacks. 0.0x disables DOT from energy entirely.</t>
         </is>
       </c>
       <c r="G13" t="inlineStr"/>
@@ -859,11 +859,11 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>OptionArmEnabled</t>
+          <t>OptionThroatEnabled</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -878,7 +878,7 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Enable bleeding from arm wounds</t>
+          <t>Enable bleeding from throat wounds</t>
         </is>
       </c>
       <c r="G14" t="inlineStr"/>
@@ -890,11 +890,11 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>OptionLegEnabled</t>
+          <t>OptionHeadEnabled</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -909,7 +909,7 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Enable bleeding from leg wounds</t>
+          <t>Enable bleeding from head wounds</t>
         </is>
       </c>
       <c r="G15" t="inlineStr"/>
@@ -921,11 +921,11 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>70</v>
+        <v>30</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>OptionDismembermentEnabled</t>
+          <t>OptionNeckEnabled</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -940,7 +940,7 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Enable bleeding from dismemberment</t>
+          <t>Enable bleeding from neck wounds</t>
         </is>
       </c>
       <c r="G16" t="inlineStr"/>
@@ -948,30 +948,30 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>CategoryZoneThroat</t>
+          <t>CategoryZoneToggles</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>OptionThroatChance</t>
+          <t>OptionTorsoEnabled</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>float</t>
+          <t>bool</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>60f</t>
+          <t>true</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Chance for throat wounds to cause bleeding</t>
+          <t>Enable bleeding from torso wounds</t>
         </is>
       </c>
       <c r="G17" t="inlineStr"/>
@@ -979,30 +979,30 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>CategoryZoneThroat</t>
+          <t>CategoryZoneToggles</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>OptionThroatDamage</t>
+          <t>OptionArmEnabled</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>float</t>
+          <t>bool</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>2.5f</t>
+          <t>true</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Base damage per tick for throat wounds</t>
+          <t>Enable bleeding from arm wounds</t>
         </is>
       </c>
       <c r="G18" t="inlineStr"/>
@@ -1010,30 +1010,30 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>CategoryZoneThroat</t>
+          <t>CategoryZoneToggles</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>OptionThroatDuration</t>
+          <t>OptionLegEnabled</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>float</t>
+          <t>bool</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>6.0f</t>
+          <t>true</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>How long throat bleeds last</t>
+          <t>Enable bleeding from leg wounds</t>
         </is>
       </c>
       <c r="G19" t="inlineStr"/>
@@ -1041,30 +1041,30 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>CategoryZoneThroat</t>
+          <t>CategoryZoneToggles</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>35</v>
+        <v>70</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>OptionThroatFrequency</t>
+          <t>OptionDismembermentEnabled</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>float</t>
+          <t>bool</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>0.5f</t>
+          <t>true</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Time between bleed ticks for throat wounds</t>
+          <t>Enable bleeding from dismemberment</t>
         </is>
       </c>
       <c r="G20" t="inlineStr"/>
@@ -1076,26 +1076,26 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>OptionThroatStackLimit</t>
+          <t>OptionThroatChance</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>int</t>
+          <t>float</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>60f</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Max stacks for throat wounds</t>
+          <t>Chance for throat wounds to cause bleeding</t>
         </is>
       </c>
       <c r="G21" t="inlineStr"/>
@@ -1103,15 +1103,15 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>CategoryZoneHead</t>
+          <t>CategoryZoneThroat</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>OptionHeadChance</t>
+          <t>OptionThroatDamage</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -1121,12 +1121,12 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>40f</t>
+          <t>2.5f</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Chance for head wounds to cause bleeding</t>
+          <t>Base damage per tick for throat wounds</t>
         </is>
       </c>
       <c r="G22" t="inlineStr"/>
@@ -1134,15 +1134,15 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>CategoryZoneHead</t>
+          <t>CategoryZoneThroat</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>OptionHeadDamage</t>
+          <t>OptionThroatDuration</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -1152,12 +1152,12 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>1.5f</t>
+          <t>6.0f</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Base damage per tick for head wounds</t>
+          <t>How long throat bleeds last</t>
         </is>
       </c>
       <c r="G23" t="inlineStr"/>
@@ -1165,15 +1165,15 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>CategoryZoneHead</t>
+          <t>CategoryZoneThroat</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>OptionHeadDuration</t>
+          <t>OptionThroatFrequency</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -1183,12 +1183,12 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>5.0f</t>
+          <t>0.5f</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>How long head bleeds last</t>
+          <t>Time between bleed ticks for throat wounds</t>
         </is>
       </c>
       <c r="G24" t="inlineStr"/>
@@ -1196,30 +1196,30 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>CategoryZoneHead</t>
+          <t>CategoryZoneThroat</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>OptionHeadFrequency</t>
+          <t>OptionThroatStackLimit</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>float</t>
+          <t>int</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>0.5f</t>
+          <t>3</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Time between bleed ticks for head wounds</t>
+          <t>Max stacks for throat wounds</t>
         </is>
       </c>
       <c r="G25" t="inlineStr"/>
@@ -1231,26 +1231,26 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>OptionHeadStackLimit</t>
+          <t>OptionHeadChance</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>int</t>
+          <t>float</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>40f</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Max stacks for head wounds</t>
+          <t>Chance for head wounds to cause bleeding</t>
         </is>
       </c>
       <c r="G26" t="inlineStr"/>
@@ -1258,15 +1258,15 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>CategoryZoneNeck</t>
+          <t>CategoryZoneHead</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>OptionNeckChance</t>
+          <t>OptionHeadDamage</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1276,12 +1276,12 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>55f</t>
+          <t>1.5f</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Chance for neck wounds to cause bleeding</t>
+          <t>Base damage per tick for head wounds</t>
         </is>
       </c>
       <c r="G27" t="inlineStr"/>
@@ -1289,15 +1289,15 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>CategoryZoneNeck</t>
+          <t>CategoryZoneHead</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>OptionNeckDamage</t>
+          <t>OptionHeadDuration</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1307,12 +1307,12 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>2.0f</t>
+          <t>5.0f</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>Base damage per tick for neck wounds</t>
+          <t>How long head bleeds last</t>
         </is>
       </c>
       <c r="G28" t="inlineStr"/>
@@ -1320,15 +1320,15 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>CategoryZoneNeck</t>
+          <t>CategoryZoneHead</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>OptionNeckDuration</t>
+          <t>OptionHeadFrequency</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -1338,12 +1338,12 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>5.5f</t>
+          <t>0.5f</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>How long neck bleeds last</t>
+          <t>Time between bleed ticks for head wounds</t>
         </is>
       </c>
       <c r="G29" t="inlineStr"/>
@@ -1351,30 +1351,30 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>CategoryZoneNeck</t>
+          <t>CategoryZoneHead</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>OptionNeckFrequency</t>
+          <t>OptionHeadStackLimit</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>float</t>
+          <t>int</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>0.5f</t>
+          <t>3</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Time between bleed ticks for neck wounds</t>
+          <t>Max stacks for head wounds</t>
         </is>
       </c>
       <c r="G30" t="inlineStr"/>
@@ -1386,26 +1386,26 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>OptionNeckStackLimit</t>
+          <t>OptionNeckChance</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>int</t>
+          <t>float</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>55f</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>Max stacks for neck wounds</t>
+          <t>Chance for neck wounds to cause bleeding</t>
         </is>
       </c>
       <c r="G31" t="inlineStr"/>
@@ -1413,15 +1413,15 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>CategoryZoneTorso</t>
+          <t>CategoryZoneNeck</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>OptionTorsoChance</t>
+          <t>OptionNeckDamage</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1431,12 +1431,12 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>35f</t>
+          <t>2.0f</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>Chance for torso wounds to cause bleeding</t>
+          <t>Base damage per tick for neck wounds</t>
         </is>
       </c>
       <c r="G32" t="inlineStr"/>
@@ -1444,15 +1444,15 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>CategoryZoneTorso</t>
+          <t>CategoryZoneNeck</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>OptionTorsoDamage</t>
+          <t>OptionNeckDuration</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -1462,12 +1462,12 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>1.0f</t>
+          <t>5.5f</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>Base damage per tick for torso wounds</t>
+          <t>How long neck bleeds last</t>
         </is>
       </c>
       <c r="G33" t="inlineStr"/>
@@ -1475,15 +1475,15 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>CategoryZoneTorso</t>
+          <t>CategoryZoneNeck</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>OptionTorsoDuration</t>
+          <t>OptionNeckFrequency</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -1493,12 +1493,12 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>4.0f</t>
+          <t>0.5f</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>How long torso bleeds last</t>
+          <t>Time between bleed ticks for neck wounds</t>
         </is>
       </c>
       <c r="G34" t="inlineStr"/>
@@ -1506,30 +1506,30 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>CategoryZoneTorso</t>
+          <t>CategoryZoneNeck</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>OptionTorsoFrequency</t>
+          <t>OptionNeckStackLimit</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>float</t>
+          <t>int</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>0.5f</t>
+          <t>3</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>Time between bleed ticks for torso wounds</t>
+          <t>Max stacks for neck wounds</t>
         </is>
       </c>
       <c r="G35" t="inlineStr"/>
@@ -1541,26 +1541,26 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>OptionTorsoStackLimit</t>
+          <t>OptionTorsoChance</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>int</t>
+          <t>float</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>35f</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>Max stacks for torso wounds</t>
+          <t>Chance for torso wounds to cause bleeding</t>
         </is>
       </c>
       <c r="G36" t="inlineStr"/>
@@ -1568,15 +1568,15 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>CategoryZoneArm</t>
+          <t>CategoryZoneTorso</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>OptionArmChance</t>
+          <t>OptionTorsoDamage</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -1586,12 +1586,12 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>25f</t>
+          <t>1.0f</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>Chance for arm wounds to cause bleeding</t>
+          <t>Base damage per tick for torso wounds</t>
         </is>
       </c>
       <c r="G37" t="inlineStr"/>
@@ -1599,15 +1599,15 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>CategoryZoneArm</t>
+          <t>CategoryZoneTorso</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>OptionArmDamage</t>
+          <t>OptionTorsoDuration</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -1617,12 +1617,12 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>0.5f</t>
+          <t>4.0f</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>Base damage per tick for arm wounds</t>
+          <t>How long torso bleeds last</t>
         </is>
       </c>
       <c r="G38" t="inlineStr"/>
@@ -1630,15 +1630,15 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>CategoryZoneArm</t>
+          <t>CategoryZoneTorso</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>OptionArmDuration</t>
+          <t>OptionTorsoFrequency</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -1648,12 +1648,12 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>3.0f</t>
+          <t>0.5f</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>How long arm bleeds last</t>
+          <t>Time between bleed ticks for torso wounds</t>
         </is>
       </c>
       <c r="G39" t="inlineStr"/>
@@ -1661,30 +1661,30 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>CategoryZoneArm</t>
+          <t>CategoryZoneTorso</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>OptionArmFrequency</t>
+          <t>OptionTorsoStackLimit</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>float</t>
+          <t>int</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>0.5f</t>
+          <t>5</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>Time between bleed ticks for arm wounds</t>
+          <t>Max stacks for torso wounds</t>
         </is>
       </c>
       <c r="G40" t="inlineStr"/>
@@ -1696,26 +1696,26 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>OptionArmStackLimit</t>
+          <t>OptionArmChance</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>int</t>
+          <t>float</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>25f</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>Max stacks for arm wounds</t>
+          <t>Chance for arm wounds to cause bleeding</t>
         </is>
       </c>
       <c r="G41" t="inlineStr"/>
@@ -1723,15 +1723,15 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>CategoryZoneLeg</t>
+          <t>CategoryZoneArm</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>OptionLegChance</t>
+          <t>OptionArmDamage</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -1741,12 +1741,12 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>30f</t>
+          <t>0.5f</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>Chance for leg wounds to cause bleeding</t>
+          <t>Base damage per tick for arm wounds</t>
         </is>
       </c>
       <c r="G42" t="inlineStr"/>
@@ -1754,15 +1754,15 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>CategoryZoneLeg</t>
+          <t>CategoryZoneArm</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>OptionLegDamage</t>
+          <t>OptionArmDuration</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -1772,12 +1772,12 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>0.75f</t>
+          <t>3.0f</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>Base damage per tick for leg wounds</t>
+          <t>How long arm bleeds last</t>
         </is>
       </c>
       <c r="G43" t="inlineStr"/>
@@ -1785,15 +1785,15 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>CategoryZoneLeg</t>
+          <t>CategoryZoneArm</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>OptionLegDuration</t>
+          <t>OptionArmFrequency</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -1803,12 +1803,12 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>3.5f</t>
+          <t>0.5f</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>How long leg bleeds last</t>
+          <t>Time between bleed ticks for arm wounds</t>
         </is>
       </c>
       <c r="G44" t="inlineStr"/>
@@ -1816,30 +1816,30 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>CategoryZoneLeg</t>
+          <t>CategoryZoneArm</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>OptionLegFrequency</t>
+          <t>OptionArmStackLimit</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>float</t>
+          <t>int</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>0.5f</t>
+          <t>4</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>Time between bleed ticks for leg wounds</t>
+          <t>Max stacks for arm wounds</t>
         </is>
       </c>
       <c r="G45" t="inlineStr"/>
@@ -1851,26 +1851,26 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>OptionLegStackLimit</t>
+          <t>OptionLegChance</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>int</t>
+          <t>float</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>30f</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>Max stacks for leg wounds</t>
+          <t>Chance for leg wounds to cause bleeding</t>
         </is>
       </c>
       <c r="G46" t="inlineStr"/>
@@ -1878,15 +1878,15 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>CategoryZoneDismemberment</t>
+          <t>CategoryZoneLeg</t>
         </is>
       </c>
       <c r="B47" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>OptionDismembermentChance</t>
+          <t>OptionLegDamage</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -1896,12 +1896,12 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>80f</t>
+          <t>0.75f</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>Chance for dismemberment to cause bleeding</t>
+          <t>Base damage per tick for leg wounds</t>
         </is>
       </c>
       <c r="G47" t="inlineStr"/>
@@ -1909,15 +1909,15 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>CategoryZoneDismemberment</t>
+          <t>CategoryZoneLeg</t>
         </is>
       </c>
       <c r="B48" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>OptionDismembermentDamage</t>
+          <t>OptionLegDuration</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -1927,12 +1927,12 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>3.0f</t>
+          <t>3.5f</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>Base damage per tick for dismemberment</t>
+          <t>How long leg bleeds last</t>
         </is>
       </c>
       <c r="G48" t="inlineStr"/>
@@ -1940,15 +1940,15 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>CategoryZoneDismemberment</t>
+          <t>CategoryZoneLeg</t>
         </is>
       </c>
       <c r="B49" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>OptionDismembermentDuration</t>
+          <t>OptionLegFrequency</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -1958,12 +1958,12 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>8.0f</t>
+          <t>0.5f</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>How long dismemberment bleeds last</t>
+          <t>Time between bleed ticks for leg wounds</t>
         </is>
       </c>
       <c r="G49" t="inlineStr"/>
@@ -1971,30 +1971,30 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>CategoryZoneDismemberment</t>
+          <t>CategoryZoneLeg</t>
         </is>
       </c>
       <c r="B50" t="n">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>OptionDismembermentFrequency</t>
+          <t>OptionLegStackLimit</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>float</t>
+          <t>int</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>0.5f</t>
+          <t>4</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>Time between bleed ticks for dismemberment</t>
+          <t>Max stacks for leg wounds</t>
         </is>
       </c>
       <c r="G50" t="inlineStr"/>
@@ -2006,26 +2006,26 @@
         </is>
       </c>
       <c r="B51" t="n">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>OptionDismembermentStackLimit</t>
+          <t>OptionDismembermentChance</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>int</t>
+          <t>float</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>80f</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>Max stacks for dismemberment (per limb)</t>
+          <t>Chance for dismemberment to cause bleeding</t>
         </is>
       </c>
       <c r="G51" t="inlineStr"/>
@@ -2033,30 +2033,30 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>CategoryAdvanced</t>
+          <t>CategoryZoneDismemberment</t>
         </is>
       </c>
       <c r="B52" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>OptionDebugLogging</t>
+          <t>OptionDismembermentDamage</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>bool</t>
+          <t>float</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>false</t>
+          <t>3.0f</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>Enable verbose debug logging</t>
+          <t>Base damage per tick for dismemberment</t>
         </is>
       </c>
       <c r="G52" t="inlineStr"/>
@@ -2064,33 +2064,157 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
+          <t>CategoryZoneDismemberment</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>30</v>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>OptionDismembermentDuration</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>float</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>8.0f</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>How long dismemberment bleeds last</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr"/>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>CategoryZoneDismemberment</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>35</v>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>OptionDismembermentFrequency</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>float</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>0.5f</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>Time between bleed ticks for dismemberment</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr"/>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>CategoryZoneDismemberment</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>40</v>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>OptionDismembermentStackLimit</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>int</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>Max stacks for dismemberment (per limb)</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr"/>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>CategoryAdvanced</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
+        <v>10</v>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>OptionDebugLogging</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>bool</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>Enable verbose debug logging</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr"/>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
           <t>CategoryStatistics</t>
         </is>
       </c>
-      <c r="B53" t="n">
+      <c r="B57" t="n">
         <v>10</v>
       </c>
-      <c r="C53" t="inlineStr">
+      <c r="C57" t="inlineStr">
         <is>
           <t>OptionResetStats</t>
         </is>
       </c>
-      <c r="D53" t="inlineStr">
+      <c r="D57" t="inlineStr">
         <is>
           <t>bool</t>
         </is>
       </c>
-      <c r="E53" t="inlineStr">
+      <c r="E57" t="inlineStr">
         <is>
           <t>false</t>
         </is>
       </c>
-      <c r="F53" t="inlineStr">
+      <c r="F57" t="inlineStr">
         <is>
           <t>Toggle to reset all statistics</t>
         </is>
       </c>
-      <c r="G53" t="inlineStr"/>
+      <c r="G57" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Remove Fire/Lightning/Energy damage type multipliers - elemental DOT is now status-only
- Removed OptionFireMultiplier, OptionLightningMultiplier, OptionEnergyMultiplier constants
- Removed FireMultiplier, LightningMultiplier, EnergyMultiplier ModOption fields
- Updated GetDamageTypeMultiplier() to only return multipliers for physical types (Pierce/Slash/Blunt)
- Simplified IsDamageTypeAllowed() to only allow physical damage types for zone-based DOT
- Updated CheckAndSyncProfileMultipliers():
  - BleedOnly now disables status multipliers (Burning/Electrocute)
  - ElementalOnly still disables physical multipliers
- Elemental damage DOT is now exclusively handled by Burning/Electrocute status effects
- Menu options reduced from 58 to 55
</commit_message>
<xml_diff>
--- a/MENU_MOCK.xlsx
+++ b/MENU_MOCK.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G57"/>
+  <dimension ref="A1:G56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -718,7 +718,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>1.0f</t>
+          <t>0.8f</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -766,11 +766,11 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>OptionFireMultiplier</t>
+          <t>OptionBurningMultiplier</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -780,12 +780,12 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>1.0f</t>
+          <t>0.5f</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>DOT damage multiplier for fire attacks. 0.0x disables DOT from fire entirely.</t>
+          <t>Additional DOT damage multiplier when creature has Burning status. Stacks with Fire multiplier. 0.0x = no bonus damage from burning status.</t>
         </is>
       </c>
       <c r="G11" t="inlineStr"/>
@@ -797,11 +797,11 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>OptionLightningMultiplier</t>
+          <t>OptionElectrocuteMultiplier</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -811,12 +811,12 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>1.0f</t>
+          <t>0.8f</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>DOT damage multiplier for lightning attacks. 0.0x disables DOT from lightning entirely.</t>
+          <t>DOT damage multiplier when creature has Electrocute status. Electrocute normally does no damage. 0.0x = no damage from electrocute.</t>
         </is>
       </c>
       <c r="G12" t="inlineStr"/>
@@ -824,30 +824,30 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>CategoryDamageTypeMultipliers</t>
+          <t>CategoryZoneToggles</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>60</v>
+        <v>10</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>OptionEnergyMultiplier</t>
+          <t>OptionThroatEnabled</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>float</t>
+          <t>bool</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>1.0f</t>
+          <t>true</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>DOT damage multiplier for energy attacks. 0.0x disables DOT from energy entirely.</t>
+          <t>Enable bleeding from throat wounds</t>
         </is>
       </c>
       <c r="G13" t="inlineStr"/>
@@ -859,11 +859,11 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>OptionThroatEnabled</t>
+          <t>OptionHeadEnabled</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -878,7 +878,7 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Enable bleeding from throat wounds</t>
+          <t>Enable bleeding from head wounds</t>
         </is>
       </c>
       <c r="G14" t="inlineStr"/>
@@ -890,11 +890,11 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>OptionHeadEnabled</t>
+          <t>OptionNeckEnabled</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -909,7 +909,7 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Enable bleeding from head wounds</t>
+          <t>Enable bleeding from neck wounds</t>
         </is>
       </c>
       <c r="G15" t="inlineStr"/>
@@ -921,11 +921,11 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>OptionNeckEnabled</t>
+          <t>OptionTorsoEnabled</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -940,7 +940,7 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Enable bleeding from neck wounds</t>
+          <t>Enable bleeding from torso wounds</t>
         </is>
       </c>
       <c r="G16" t="inlineStr"/>
@@ -952,11 +952,11 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>OptionTorsoEnabled</t>
+          <t>OptionArmEnabled</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -971,7 +971,7 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Enable bleeding from torso wounds</t>
+          <t>Enable bleeding from arm wounds</t>
         </is>
       </c>
       <c r="G17" t="inlineStr"/>
@@ -983,11 +983,11 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>OptionArmEnabled</t>
+          <t>OptionLegEnabled</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1002,7 +1002,7 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Enable bleeding from arm wounds</t>
+          <t>Enable bleeding from leg wounds</t>
         </is>
       </c>
       <c r="G18" t="inlineStr"/>
@@ -1014,11 +1014,11 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>OptionLegEnabled</t>
+          <t>OptionDismembermentEnabled</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -1033,7 +1033,7 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Enable bleeding from leg wounds</t>
+          <t>Enable bleeding from dismemberment</t>
         </is>
       </c>
       <c r="G19" t="inlineStr"/>
@@ -1041,30 +1041,30 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>CategoryZoneToggles</t>
+          <t>CategoryZoneThroat</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>OptionDismembermentEnabled</t>
+          <t>OptionThroatChance</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>bool</t>
+          <t>float</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>true</t>
+          <t>60f</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Enable bleeding from dismemberment</t>
+          <t>Chance for throat wounds to cause bleeding</t>
         </is>
       </c>
       <c r="G20" t="inlineStr"/>
@@ -1076,11 +1076,11 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>OptionThroatChance</t>
+          <t>OptionThroatDamage</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1090,12 +1090,12 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>60f</t>
+          <t>2.5f</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Chance for throat wounds to cause bleeding</t>
+          <t>Base damage per tick for throat wounds</t>
         </is>
       </c>
       <c r="G21" t="inlineStr"/>
@@ -1107,11 +1107,11 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>OptionThroatDamage</t>
+          <t>OptionThroatDuration</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -1121,12 +1121,12 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>2.5f</t>
+          <t>6.0f</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Base damage per tick for throat wounds</t>
+          <t>How long throat bleeds last</t>
         </is>
       </c>
       <c r="G22" t="inlineStr"/>
@@ -1138,11 +1138,11 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>OptionThroatDuration</t>
+          <t>OptionThroatFrequency</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -1152,12 +1152,12 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>6.0f</t>
+          <t>0.5f</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>How long throat bleeds last</t>
+          <t>Time between bleed ticks for throat wounds</t>
         </is>
       </c>
       <c r="G23" t="inlineStr"/>
@@ -1169,26 +1169,26 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>OptionThroatFrequency</t>
+          <t>OptionThroatStackLimit</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>float</t>
+          <t>int</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>0.5f</t>
+          <t>3</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Time between bleed ticks for throat wounds</t>
+          <t>Max stacks for throat wounds</t>
         </is>
       </c>
       <c r="G24" t="inlineStr"/>
@@ -1196,30 +1196,30 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>CategoryZoneThroat</t>
+          <t>CategoryZoneHead</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>OptionThroatStackLimit</t>
+          <t>OptionHeadChance</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>int</t>
+          <t>float</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>40f</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Max stacks for throat wounds</t>
+          <t>Chance for head wounds to cause bleeding</t>
         </is>
       </c>
       <c r="G25" t="inlineStr"/>
@@ -1231,11 +1231,11 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>OptionHeadChance</t>
+          <t>OptionHeadDamage</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1245,12 +1245,12 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>40f</t>
+          <t>1.5f</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Chance for head wounds to cause bleeding</t>
+          <t>Base damage per tick for head wounds</t>
         </is>
       </c>
       <c r="G26" t="inlineStr"/>
@@ -1262,11 +1262,11 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>OptionHeadDamage</t>
+          <t>OptionHeadDuration</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1276,12 +1276,12 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>1.5f</t>
+          <t>5.0f</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Base damage per tick for head wounds</t>
+          <t>How long head bleeds last</t>
         </is>
       </c>
       <c r="G27" t="inlineStr"/>
@@ -1293,11 +1293,11 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>OptionHeadDuration</t>
+          <t>OptionHeadFrequency</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1307,12 +1307,12 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>5.0f</t>
+          <t>0.5f</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>How long head bleeds last</t>
+          <t>Time between bleed ticks for head wounds</t>
         </is>
       </c>
       <c r="G28" t="inlineStr"/>
@@ -1324,26 +1324,26 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>OptionHeadFrequency</t>
+          <t>OptionHeadStackLimit</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>float</t>
+          <t>int</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>0.5f</t>
+          <t>3</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Time between bleed ticks for head wounds</t>
+          <t>Max stacks for head wounds</t>
         </is>
       </c>
       <c r="G29" t="inlineStr"/>
@@ -1351,30 +1351,30 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>CategoryZoneHead</t>
+          <t>CategoryZoneNeck</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>OptionHeadStackLimit</t>
+          <t>OptionNeckChance</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>int</t>
+          <t>float</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>55f</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Max stacks for head wounds</t>
+          <t>Chance for neck wounds to cause bleeding</t>
         </is>
       </c>
       <c r="G30" t="inlineStr"/>
@@ -1386,11 +1386,11 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>OptionNeckChance</t>
+          <t>OptionNeckDamage</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1400,12 +1400,12 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>55f</t>
+          <t>2.0f</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>Chance for neck wounds to cause bleeding</t>
+          <t>Base damage per tick for neck wounds</t>
         </is>
       </c>
       <c r="G31" t="inlineStr"/>
@@ -1417,11 +1417,11 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>OptionNeckDamage</t>
+          <t>OptionNeckDuration</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1431,12 +1431,12 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>2.0f</t>
+          <t>5.5f</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>Base damage per tick for neck wounds</t>
+          <t>How long neck bleeds last</t>
         </is>
       </c>
       <c r="G32" t="inlineStr"/>
@@ -1448,11 +1448,11 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>OptionNeckDuration</t>
+          <t>OptionNeckFrequency</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -1462,12 +1462,12 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>5.5f</t>
+          <t>0.5f</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>How long neck bleeds last</t>
+          <t>Time between bleed ticks for neck wounds</t>
         </is>
       </c>
       <c r="G33" t="inlineStr"/>
@@ -1479,26 +1479,26 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>OptionNeckFrequency</t>
+          <t>OptionNeckStackLimit</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>float</t>
+          <t>int</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>0.5f</t>
+          <t>3</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Time between bleed ticks for neck wounds</t>
+          <t>Max stacks for neck wounds</t>
         </is>
       </c>
       <c r="G34" t="inlineStr"/>
@@ -1506,30 +1506,30 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>CategoryZoneNeck</t>
+          <t>CategoryZoneTorso</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>OptionNeckStackLimit</t>
+          <t>OptionTorsoChance</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>int</t>
+          <t>float</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>35f</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>Max stacks for neck wounds</t>
+          <t>Chance for torso wounds to cause bleeding</t>
         </is>
       </c>
       <c r="G35" t="inlineStr"/>
@@ -1541,11 +1541,11 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>OptionTorsoChance</t>
+          <t>OptionTorsoDamage</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -1555,12 +1555,12 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>35f</t>
+          <t>1.0f</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>Chance for torso wounds to cause bleeding</t>
+          <t>Base damage per tick for torso wounds</t>
         </is>
       </c>
       <c r="G36" t="inlineStr"/>
@@ -1572,11 +1572,11 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>OptionTorsoDamage</t>
+          <t>OptionTorsoDuration</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -1586,12 +1586,12 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>1.0f</t>
+          <t>4.0f</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>Base damage per tick for torso wounds</t>
+          <t>How long torso bleeds last</t>
         </is>
       </c>
       <c r="G37" t="inlineStr"/>
@@ -1603,11 +1603,11 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>OptionTorsoDuration</t>
+          <t>OptionTorsoFrequency</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -1617,12 +1617,12 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>4.0f</t>
+          <t>0.5f</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>How long torso bleeds last</t>
+          <t>Time between bleed ticks for torso wounds</t>
         </is>
       </c>
       <c r="G38" t="inlineStr"/>
@@ -1634,26 +1634,26 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>OptionTorsoFrequency</t>
+          <t>OptionTorsoStackLimit</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>float</t>
+          <t>int</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>0.5f</t>
+          <t>5</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>Time between bleed ticks for torso wounds</t>
+          <t>Max stacks for torso wounds</t>
         </is>
       </c>
       <c r="G39" t="inlineStr"/>
@@ -1661,30 +1661,30 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>CategoryZoneTorso</t>
+          <t>CategoryZoneArm</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>OptionTorsoStackLimit</t>
+          <t>OptionArmChance</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>int</t>
+          <t>float</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>25f</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>Max stacks for torso wounds</t>
+          <t>Chance for arm wounds to cause bleeding</t>
         </is>
       </c>
       <c r="G40" t="inlineStr"/>
@@ -1696,11 +1696,11 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>OptionArmChance</t>
+          <t>OptionArmDamage</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -1710,12 +1710,12 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>25f</t>
+          <t>0.5f</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>Chance for arm wounds to cause bleeding</t>
+          <t>Base damage per tick for arm wounds</t>
         </is>
       </c>
       <c r="G41" t="inlineStr"/>
@@ -1727,11 +1727,11 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>OptionArmDamage</t>
+          <t>OptionArmDuration</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -1741,12 +1741,12 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>0.5f</t>
+          <t>3.0f</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>Base damage per tick for arm wounds</t>
+          <t>How long arm bleeds last</t>
         </is>
       </c>
       <c r="G42" t="inlineStr"/>
@@ -1758,11 +1758,11 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>OptionArmDuration</t>
+          <t>OptionArmFrequency</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -1772,12 +1772,12 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>3.0f</t>
+          <t>0.5f</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>How long arm bleeds last</t>
+          <t>Time between bleed ticks for arm wounds</t>
         </is>
       </c>
       <c r="G43" t="inlineStr"/>
@@ -1789,26 +1789,26 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>OptionArmFrequency</t>
+          <t>OptionArmStackLimit</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>float</t>
+          <t>int</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>0.5f</t>
+          <t>4</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>Time between bleed ticks for arm wounds</t>
+          <t>Max stacks for arm wounds</t>
         </is>
       </c>
       <c r="G44" t="inlineStr"/>
@@ -1816,30 +1816,30 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>CategoryZoneArm</t>
+          <t>CategoryZoneLeg</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>OptionArmStackLimit</t>
+          <t>OptionLegChance</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>int</t>
+          <t>float</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>30f</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>Max stacks for arm wounds</t>
+          <t>Chance for leg wounds to cause bleeding</t>
         </is>
       </c>
       <c r="G45" t="inlineStr"/>
@@ -1851,11 +1851,11 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>OptionLegChance</t>
+          <t>OptionLegDamage</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -1865,12 +1865,12 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>30f</t>
+          <t>0.75f</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>Chance for leg wounds to cause bleeding</t>
+          <t>Base damage per tick for leg wounds</t>
         </is>
       </c>
       <c r="G46" t="inlineStr"/>
@@ -1882,11 +1882,11 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>OptionLegDamage</t>
+          <t>OptionLegDuration</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -1896,12 +1896,12 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>0.75f</t>
+          <t>3.5f</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>Base damage per tick for leg wounds</t>
+          <t>How long leg bleeds last</t>
         </is>
       </c>
       <c r="G47" t="inlineStr"/>
@@ -1913,11 +1913,11 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>OptionLegDuration</t>
+          <t>OptionLegFrequency</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -1927,12 +1927,12 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>3.5f</t>
+          <t>0.5f</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>How long leg bleeds last</t>
+          <t>Time between bleed ticks for leg wounds</t>
         </is>
       </c>
       <c r="G48" t="inlineStr"/>
@@ -1944,26 +1944,26 @@
         </is>
       </c>
       <c r="B49" t="n">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>OptionLegFrequency</t>
+          <t>OptionLegStackLimit</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>float</t>
+          <t>int</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>0.5f</t>
+          <t>4</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>Time between bleed ticks for leg wounds</t>
+          <t>Max stacks for leg wounds</t>
         </is>
       </c>
       <c r="G49" t="inlineStr"/>
@@ -1971,30 +1971,30 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>CategoryZoneLeg</t>
+          <t>CategoryZoneDismemberment</t>
         </is>
       </c>
       <c r="B50" t="n">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>OptionLegStackLimit</t>
+          <t>OptionDismembermentChance</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>int</t>
+          <t>float</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>80f</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>Max stacks for leg wounds</t>
+          <t>Chance for dismemberment to cause bleeding</t>
         </is>
       </c>
       <c r="G50" t="inlineStr"/>
@@ -2006,11 +2006,11 @@
         </is>
       </c>
       <c r="B51" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>OptionDismembermentChance</t>
+          <t>OptionDismembermentDamage</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
@@ -2020,12 +2020,12 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>80f</t>
+          <t>3.0f</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>Chance for dismemberment to cause bleeding</t>
+          <t>Base damage per tick for dismemberment</t>
         </is>
       </c>
       <c r="G51" t="inlineStr"/>
@@ -2037,11 +2037,11 @@
         </is>
       </c>
       <c r="B52" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>OptionDismembermentDamage</t>
+          <t>OptionDismembermentDuration</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -2051,12 +2051,12 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>3.0f</t>
+          <t>8.0f</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>Base damage per tick for dismemberment</t>
+          <t>How long dismemberment bleeds last</t>
         </is>
       </c>
       <c r="G52" t="inlineStr"/>
@@ -2068,11 +2068,11 @@
         </is>
       </c>
       <c r="B53" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>OptionDismembermentDuration</t>
+          <t>OptionDismembermentFrequency</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -2082,12 +2082,12 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>8.0f</t>
+          <t>0.5f</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>How long dismemberment bleeds last</t>
+          <t>Time between bleed ticks for dismemberment</t>
         </is>
       </c>
       <c r="G53" t="inlineStr"/>
@@ -2099,26 +2099,26 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>OptionDismembermentFrequency</t>
+          <t>OptionDismembermentStackLimit</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>float</t>
+          <t>int</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>0.5f</t>
+          <t>1</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>Time between bleed ticks for dismemberment</t>
+          <t>Max stacks for dismemberment (per limb)</t>
         </is>
       </c>
       <c r="G54" t="inlineStr"/>
@@ -2126,30 +2126,30 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>CategoryZoneDismemberment</t>
+          <t>CategoryAdvanced</t>
         </is>
       </c>
       <c r="B55" t="n">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>OptionDismembermentStackLimit</t>
+          <t>OptionDebugLogging</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>int</t>
+          <t>bool</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>false</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>Max stacks for dismemberment (per limb)</t>
+          <t>Enable verbose debug logging</t>
         </is>
       </c>
       <c r="G55" t="inlineStr"/>
@@ -2157,7 +2157,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>CategoryAdvanced</t>
+          <t>CategoryStatistics</t>
         </is>
       </c>
       <c r="B56" t="n">
@@ -2165,7 +2165,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>OptionDebugLogging</t>
+          <t>OptionResetStats</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -2180,41 +2180,10 @@
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>Enable verbose debug logging</t>
+          <t>Toggle to reset all statistics</t>
         </is>
       </c>
       <c r="G56" t="inlineStr"/>
-    </row>
-    <row r="57">
-      <c r="A57" t="inlineStr">
-        <is>
-          <t>CategoryStatistics</t>
-        </is>
-      </c>
-      <c r="B57" t="n">
-        <v>10</v>
-      </c>
-      <c r="C57" t="inlineStr">
-        <is>
-          <t>OptionResetStats</t>
-        </is>
-      </c>
-      <c r="D57" t="inlineStr">
-        <is>
-          <t>bool</t>
-        </is>
-      </c>
-      <c r="E57" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="F57" t="inlineStr">
-        <is>
-          <t>Toggle to reset all statistics</t>
-        </is>
-      </c>
-      <c r="G57" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Unify elemental DOT to zone-based system with visual status effects
- Fire/Lightning now use zone-based DOT (like Pierce/Slash/Blunt)
- Replaced BurningStatusMultiplier/ElectrocuteStatusMultiplier with FireMultiplier/LightningMultiplier
- Fire DOT applies Burning visual via creature.Inflict() during ticks
- Lightning DOT applies Electrocute visual via creature.Inflict() during ticks
- Visual status effects maintained while DOT active, fade naturally when DOT ends
- Removed ApplyStatusEffectDamage() - all damage is now zone-based
- Profile sync: BleedOnly disables Fire/Lightning, ElementalOnly disables Pierce/Slash/Blunt

DOT System now unified:
- All damage types (physical + elemental) use zone-based DOT
- Elemental DOT adds visual feedback via Burning/Electrocute status
- Configurable per-zone: chance, damage, duration, frequency, stacks
</commit_message>
<xml_diff>
--- a/MENU_MOCK.xlsx
+++ b/MENU_MOCK.xlsx
@@ -766,11 +766,11 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>OptionBurningMultiplier</t>
+          <t>OptionFireMultiplier</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -780,12 +780,12 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>0.5f</t>
+          <t>1.2f</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Additional DOT damage multiplier when creature has Burning status. Stacks with Fire multiplier. 0.0x = no bonus damage from burning status.</t>
+          <t>DOT damage multiplier for fire attacks. While active, creature has Burning visual effect. 0.0x disables DOT from fire entirely.</t>
         </is>
       </c>
       <c r="G11" t="inlineStr"/>
@@ -797,11 +797,11 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>OptionElectrocuteMultiplier</t>
+          <t>OptionLightningMultiplier</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -811,12 +811,12 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>0.8f</t>
+          <t>1.2f</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>DOT damage multiplier when creature has Electrocute status. Electrocute normally does no damage. 0.0x = no damage from electrocute.</t>
+          <t>DOT damage multiplier for lightning attacks. While active, creature has Electrocute visual effect. 0.0x disables DOT from lightning entirely.</t>
         </is>
       </c>
       <c r="G12" t="inlineStr"/>

</xml_diff>

<commit_message>
Add Blood Amount preset and fix damage type multiplier defaults - Add Blood Amount preset: Very Low (0.25x), Low (0.5x), Default (1.0x), High (1.5x), Extreme (2.0x) - Update damage type multiplier defaults to match screenshot:   Pierce=1.2x, Slash=0.8x, Blunt=0.5x, Fire=0.6x, Lightning=1.5x - Apply blood amount multiplier to VFX intensity in BleedManager
</commit_message>
<xml_diff>
--- a/MENU_MOCK.xlsx
+++ b/MENU_MOCK.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G56"/>
+  <dimension ref="A1:G57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -669,30 +669,30 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>CategoryDamageTypeMultipliers</t>
+          <t>CategoryPresetSelection</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>OptionPierceMultiplier</t>
+          <t>OptionBloodAmountPreset</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>float</t>
+          <t>string</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1.0f</t>
+          <t>"Default"</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>DOT damage multiplier for pierce attacks. 0.0x disables DOT from pierce entirely.</t>
+          <t>Blood VFX intensity preset. Controls how much blood spurts from wounds. Very Low = minimal blood, Default = moderate blood, Extreme = lots of blood.</t>
         </is>
       </c>
       <c r="G8" t="inlineStr"/>
@@ -704,11 +704,11 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>OptionSlashMultiplier</t>
+          <t>OptionPierceMultiplier</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -718,12 +718,12 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>0.8f</t>
+          <t>1.2f</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>DOT damage multiplier for slash attacks. 0.0x disables DOT from slash entirely.</t>
+          <t>DOT damage multiplier for pierce attacks. 0.0x disables DOT from pierce entirely.</t>
         </is>
       </c>
       <c r="G9" t="inlineStr"/>
@@ -735,11 +735,11 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>OptionBluntMultiplier</t>
+          <t>OptionSlashMultiplier</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -749,12 +749,12 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>0.5f</t>
+          <t>0.8f</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>DOT damage multiplier for blunt attacks. 0.0x disables DOT from blunt entirely.</t>
+          <t>DOT damage multiplier for slash attacks. 0.0x disables DOT from slash entirely.</t>
         </is>
       </c>
       <c r="G10" t="inlineStr"/>
@@ -766,11 +766,11 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>OptionFireMultiplier</t>
+          <t>OptionBluntMultiplier</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -780,12 +780,12 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>1.2f</t>
+          <t>0.5f</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>DOT damage multiplier for fire attacks. While active, creature has Burning visual effect. 0.0x disables DOT from fire entirely.</t>
+          <t>DOT damage multiplier for blunt attacks. 0.0x disables DOT from blunt entirely.</t>
         </is>
       </c>
       <c r="G11" t="inlineStr"/>
@@ -797,11 +797,11 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>OptionLightningMultiplier</t>
+          <t>OptionFireMultiplier</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -811,12 +811,12 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>1.2f</t>
+          <t>0.6f</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>DOT damage multiplier for lightning attacks. While active, creature has Electrocute visual effect. 0.0x disables DOT from lightning entirely.</t>
+          <t>DOT damage multiplier for fire attacks. While active, creature has Burning visual effect. 0.0x disables DOT from fire entirely.</t>
         </is>
       </c>
       <c r="G12" t="inlineStr"/>
@@ -824,30 +824,30 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>CategoryZoneToggles</t>
+          <t>CategoryDamageTypeMultipliers</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>OptionThroatEnabled</t>
+          <t>OptionLightningMultiplier</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>bool</t>
+          <t>float</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>true</t>
+          <t>1.5f</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Enable bleeding from throat wounds</t>
+          <t>DOT damage multiplier for lightning attacks. While active, creature has Electrocute visual effect. 0.0x disables DOT from lightning entirely.</t>
         </is>
       </c>
       <c r="G13" t="inlineStr"/>
@@ -859,11 +859,11 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>OptionHeadEnabled</t>
+          <t>OptionThroatEnabled</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -878,7 +878,7 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Enable bleeding from head wounds</t>
+          <t>Enable bleeding from throat wounds</t>
         </is>
       </c>
       <c r="G14" t="inlineStr"/>
@@ -890,11 +890,11 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>OptionNeckEnabled</t>
+          <t>OptionHeadEnabled</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -909,7 +909,7 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Enable bleeding from neck wounds</t>
+          <t>Enable bleeding from head wounds</t>
         </is>
       </c>
       <c r="G15" t="inlineStr"/>
@@ -921,11 +921,11 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>OptionTorsoEnabled</t>
+          <t>OptionNeckEnabled</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -940,7 +940,7 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Enable bleeding from torso wounds</t>
+          <t>Enable bleeding from neck wounds</t>
         </is>
       </c>
       <c r="G16" t="inlineStr"/>
@@ -952,11 +952,11 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>OptionArmEnabled</t>
+          <t>OptionTorsoEnabled</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -971,7 +971,7 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Enable bleeding from arm wounds</t>
+          <t>Enable bleeding from torso wounds</t>
         </is>
       </c>
       <c r="G17" t="inlineStr"/>
@@ -983,11 +983,11 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>OptionLegEnabled</t>
+          <t>OptionArmEnabled</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1002,7 +1002,7 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Enable bleeding from leg wounds</t>
+          <t>Enable bleeding from arm wounds</t>
         </is>
       </c>
       <c r="G18" t="inlineStr"/>
@@ -1014,11 +1014,11 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>OptionDismembermentEnabled</t>
+          <t>OptionLegEnabled</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -1033,7 +1033,7 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Enable bleeding from dismemberment</t>
+          <t>Enable bleeding from leg wounds</t>
         </is>
       </c>
       <c r="G19" t="inlineStr"/>
@@ -1041,30 +1041,30 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>CategoryZoneThroat</t>
+          <t>CategoryZoneToggles</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>OptionThroatChance</t>
+          <t>OptionDismembermentEnabled</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>float</t>
+          <t>bool</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>60f</t>
+          <t>true</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Chance for throat wounds to cause bleeding</t>
+          <t>Enable bleeding from dismemberment</t>
         </is>
       </c>
       <c r="G20" t="inlineStr"/>
@@ -1076,11 +1076,11 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>OptionThroatDamage</t>
+          <t>OptionThroatChance</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1090,12 +1090,12 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>2.5f</t>
+          <t>60f</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Base damage per tick for throat wounds</t>
+          <t>Chance for throat wounds to cause bleeding</t>
         </is>
       </c>
       <c r="G21" t="inlineStr"/>
@@ -1107,11 +1107,11 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>OptionThroatDuration</t>
+          <t>OptionThroatDamage</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -1121,12 +1121,12 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>6.0f</t>
+          <t>2.5f</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>How long throat bleeds last</t>
+          <t>Base damage per tick for throat wounds</t>
         </is>
       </c>
       <c r="G22" t="inlineStr"/>
@@ -1138,11 +1138,11 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>OptionThroatFrequency</t>
+          <t>OptionThroatDuration</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -1152,12 +1152,12 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>0.5f</t>
+          <t>6.0f</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Time between bleed ticks for throat wounds</t>
+          <t>How long throat bleeds last</t>
         </is>
       </c>
       <c r="G23" t="inlineStr"/>
@@ -1169,26 +1169,26 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>OptionThroatStackLimit</t>
+          <t>OptionThroatFrequency</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>int</t>
+          <t>float</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>0.5f</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Max stacks for throat wounds</t>
+          <t>Time between bleed ticks for throat wounds</t>
         </is>
       </c>
       <c r="G24" t="inlineStr"/>
@@ -1196,30 +1196,30 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>CategoryZoneHead</t>
+          <t>CategoryZoneThroat</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>OptionHeadChance</t>
+          <t>OptionThroatStackLimit</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>float</t>
+          <t>int</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>40f</t>
+          <t>3</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Chance for head wounds to cause bleeding</t>
+          <t>Max stacks for throat wounds</t>
         </is>
       </c>
       <c r="G25" t="inlineStr"/>
@@ -1231,11 +1231,11 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>OptionHeadDamage</t>
+          <t>OptionHeadChance</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1245,12 +1245,12 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>1.5f</t>
+          <t>40f</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Base damage per tick for head wounds</t>
+          <t>Chance for head wounds to cause bleeding</t>
         </is>
       </c>
       <c r="G26" t="inlineStr"/>
@@ -1262,11 +1262,11 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>OptionHeadDuration</t>
+          <t>OptionHeadDamage</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1276,12 +1276,12 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>5.0f</t>
+          <t>1.5f</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>How long head bleeds last</t>
+          <t>Base damage per tick for head wounds</t>
         </is>
       </c>
       <c r="G27" t="inlineStr"/>
@@ -1293,11 +1293,11 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>OptionHeadFrequency</t>
+          <t>OptionHeadDuration</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1307,12 +1307,12 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>0.5f</t>
+          <t>5.0f</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>Time between bleed ticks for head wounds</t>
+          <t>How long head bleeds last</t>
         </is>
       </c>
       <c r="G28" t="inlineStr"/>
@@ -1324,26 +1324,26 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>OptionHeadStackLimit</t>
+          <t>OptionHeadFrequency</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>int</t>
+          <t>float</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>0.5f</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Max stacks for head wounds</t>
+          <t>Time between bleed ticks for head wounds</t>
         </is>
       </c>
       <c r="G29" t="inlineStr"/>
@@ -1351,30 +1351,30 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>CategoryZoneNeck</t>
+          <t>CategoryZoneHead</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>OptionNeckChance</t>
+          <t>OptionHeadStackLimit</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>float</t>
+          <t>int</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>55f</t>
+          <t>3</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Chance for neck wounds to cause bleeding</t>
+          <t>Max stacks for head wounds</t>
         </is>
       </c>
       <c r="G30" t="inlineStr"/>
@@ -1386,11 +1386,11 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>OptionNeckDamage</t>
+          <t>OptionNeckChance</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1400,12 +1400,12 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>2.0f</t>
+          <t>55f</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>Base damage per tick for neck wounds</t>
+          <t>Chance for neck wounds to cause bleeding</t>
         </is>
       </c>
       <c r="G31" t="inlineStr"/>
@@ -1417,11 +1417,11 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>OptionNeckDuration</t>
+          <t>OptionNeckDamage</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1431,12 +1431,12 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>5.5f</t>
+          <t>2.0f</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>How long neck bleeds last</t>
+          <t>Base damage per tick for neck wounds</t>
         </is>
       </c>
       <c r="G32" t="inlineStr"/>
@@ -1448,11 +1448,11 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>OptionNeckFrequency</t>
+          <t>OptionNeckDuration</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -1462,12 +1462,12 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>0.5f</t>
+          <t>5.5f</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>Time between bleed ticks for neck wounds</t>
+          <t>How long neck bleeds last</t>
         </is>
       </c>
       <c r="G33" t="inlineStr"/>
@@ -1479,26 +1479,26 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>OptionNeckStackLimit</t>
+          <t>OptionNeckFrequency</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>int</t>
+          <t>float</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>0.5f</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Max stacks for neck wounds</t>
+          <t>Time between bleed ticks for neck wounds</t>
         </is>
       </c>
       <c r="G34" t="inlineStr"/>
@@ -1506,30 +1506,30 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>CategoryZoneTorso</t>
+          <t>CategoryZoneNeck</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>OptionTorsoChance</t>
+          <t>OptionNeckStackLimit</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>float</t>
+          <t>int</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>35f</t>
+          <t>3</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>Chance for torso wounds to cause bleeding</t>
+          <t>Max stacks for neck wounds</t>
         </is>
       </c>
       <c r="G35" t="inlineStr"/>
@@ -1541,11 +1541,11 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>OptionTorsoDamage</t>
+          <t>OptionTorsoChance</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -1555,12 +1555,12 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>1.0f</t>
+          <t>35f</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>Base damage per tick for torso wounds</t>
+          <t>Chance for torso wounds to cause bleeding</t>
         </is>
       </c>
       <c r="G36" t="inlineStr"/>
@@ -1572,11 +1572,11 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>OptionTorsoDuration</t>
+          <t>OptionTorsoDamage</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -1586,12 +1586,12 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>4.0f</t>
+          <t>1.0f</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>How long torso bleeds last</t>
+          <t>Base damage per tick for torso wounds</t>
         </is>
       </c>
       <c r="G37" t="inlineStr"/>
@@ -1603,11 +1603,11 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>OptionTorsoFrequency</t>
+          <t>OptionTorsoDuration</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -1617,12 +1617,12 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>0.5f</t>
+          <t>4.0f</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>Time between bleed ticks for torso wounds</t>
+          <t>How long torso bleeds last</t>
         </is>
       </c>
       <c r="G38" t="inlineStr"/>
@@ -1634,26 +1634,26 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>OptionTorsoStackLimit</t>
+          <t>OptionTorsoFrequency</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>int</t>
+          <t>float</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>0.5f</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>Max stacks for torso wounds</t>
+          <t>Time between bleed ticks for torso wounds</t>
         </is>
       </c>
       <c r="G39" t="inlineStr"/>
@@ -1661,30 +1661,30 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>CategoryZoneArm</t>
+          <t>CategoryZoneTorso</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>OptionArmChance</t>
+          <t>OptionTorsoStackLimit</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>float</t>
+          <t>int</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>25f</t>
+          <t>5</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>Chance for arm wounds to cause bleeding</t>
+          <t>Max stacks for torso wounds</t>
         </is>
       </c>
       <c r="G40" t="inlineStr"/>
@@ -1696,11 +1696,11 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>OptionArmDamage</t>
+          <t>OptionArmChance</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -1710,12 +1710,12 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>0.5f</t>
+          <t>25f</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>Base damage per tick for arm wounds</t>
+          <t>Chance for arm wounds to cause bleeding</t>
         </is>
       </c>
       <c r="G41" t="inlineStr"/>
@@ -1727,11 +1727,11 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>OptionArmDuration</t>
+          <t>OptionArmDamage</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -1741,12 +1741,12 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>3.0f</t>
+          <t>0.5f</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>How long arm bleeds last</t>
+          <t>Base damage per tick for arm wounds</t>
         </is>
       </c>
       <c r="G42" t="inlineStr"/>
@@ -1758,11 +1758,11 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>OptionArmFrequency</t>
+          <t>OptionArmDuration</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -1772,12 +1772,12 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>0.5f</t>
+          <t>3.0f</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>Time between bleed ticks for arm wounds</t>
+          <t>How long arm bleeds last</t>
         </is>
       </c>
       <c r="G43" t="inlineStr"/>
@@ -1789,26 +1789,26 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>OptionArmStackLimit</t>
+          <t>OptionArmFrequency</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>int</t>
+          <t>float</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>0.5f</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>Max stacks for arm wounds</t>
+          <t>Time between bleed ticks for arm wounds</t>
         </is>
       </c>
       <c r="G44" t="inlineStr"/>
@@ -1816,30 +1816,30 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>CategoryZoneLeg</t>
+          <t>CategoryZoneArm</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>OptionLegChance</t>
+          <t>OptionArmStackLimit</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>float</t>
+          <t>int</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>30f</t>
+          <t>4</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>Chance for leg wounds to cause bleeding</t>
+          <t>Max stacks for arm wounds</t>
         </is>
       </c>
       <c r="G45" t="inlineStr"/>
@@ -1851,11 +1851,11 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>OptionLegDamage</t>
+          <t>OptionLegChance</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -1865,12 +1865,12 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>0.75f</t>
+          <t>30f</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>Base damage per tick for leg wounds</t>
+          <t>Chance for leg wounds to cause bleeding</t>
         </is>
       </c>
       <c r="G46" t="inlineStr"/>
@@ -1882,11 +1882,11 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>OptionLegDuration</t>
+          <t>OptionLegDamage</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -1896,12 +1896,12 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>3.5f</t>
+          <t>0.75f</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>How long leg bleeds last</t>
+          <t>Base damage per tick for leg wounds</t>
         </is>
       </c>
       <c r="G47" t="inlineStr"/>
@@ -1913,11 +1913,11 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>OptionLegFrequency</t>
+          <t>OptionLegDuration</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -1927,12 +1927,12 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>0.5f</t>
+          <t>3.5f</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>Time between bleed ticks for leg wounds</t>
+          <t>How long leg bleeds last</t>
         </is>
       </c>
       <c r="G48" t="inlineStr"/>
@@ -1944,26 +1944,26 @@
         </is>
       </c>
       <c r="B49" t="n">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>OptionLegStackLimit</t>
+          <t>OptionLegFrequency</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>int</t>
+          <t>float</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>0.5f</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>Max stacks for leg wounds</t>
+          <t>Time between bleed ticks for leg wounds</t>
         </is>
       </c>
       <c r="G49" t="inlineStr"/>
@@ -1971,30 +1971,30 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>CategoryZoneDismemberment</t>
+          <t>CategoryZoneLeg</t>
         </is>
       </c>
       <c r="B50" t="n">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>OptionDismembermentChance</t>
+          <t>OptionLegStackLimit</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>float</t>
+          <t>int</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>80f</t>
+          <t>4</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>Chance for dismemberment to cause bleeding</t>
+          <t>Max stacks for leg wounds</t>
         </is>
       </c>
       <c r="G50" t="inlineStr"/>
@@ -2006,11 +2006,11 @@
         </is>
       </c>
       <c r="B51" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>OptionDismembermentDamage</t>
+          <t>OptionDismembermentChance</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
@@ -2020,12 +2020,12 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>3.0f</t>
+          <t>80f</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>Base damage per tick for dismemberment</t>
+          <t>Chance for dismemberment to cause bleeding</t>
         </is>
       </c>
       <c r="G51" t="inlineStr"/>
@@ -2037,11 +2037,11 @@
         </is>
       </c>
       <c r="B52" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>OptionDismembermentDuration</t>
+          <t>OptionDismembermentDamage</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -2051,12 +2051,12 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>8.0f</t>
+          <t>3.0f</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>How long dismemberment bleeds last</t>
+          <t>Base damage per tick for dismemberment</t>
         </is>
       </c>
       <c r="G52" t="inlineStr"/>
@@ -2068,11 +2068,11 @@
         </is>
       </c>
       <c r="B53" t="n">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>OptionDismembermentFrequency</t>
+          <t>OptionDismembermentDuration</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -2082,12 +2082,12 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>0.5f</t>
+          <t>8.0f</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>Time between bleed ticks for dismemberment</t>
+          <t>How long dismemberment bleeds last</t>
         </is>
       </c>
       <c r="G53" t="inlineStr"/>
@@ -2099,26 +2099,26 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>OptionDismembermentStackLimit</t>
+          <t>OptionDismembermentFrequency</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>int</t>
+          <t>float</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0.5f</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>Max stacks for dismemberment (per limb)</t>
+          <t>Time between bleed ticks for dismemberment</t>
         </is>
       </c>
       <c r="G54" t="inlineStr"/>
@@ -2126,30 +2126,30 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>CategoryAdvanced</t>
+          <t>CategoryZoneDismemberment</t>
         </is>
       </c>
       <c r="B55" t="n">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>OptionDebugLogging</t>
+          <t>OptionDismembermentStackLimit</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>bool</t>
+          <t>int</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>false</t>
+          <t>1</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>Enable verbose debug logging</t>
+          <t>Max stacks for dismemberment (per limb)</t>
         </is>
       </c>
       <c r="G55" t="inlineStr"/>
@@ -2157,7 +2157,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>CategoryStatistics</t>
+          <t>CategoryAdvanced</t>
         </is>
       </c>
       <c r="B56" t="n">
@@ -2165,25 +2165,56 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
+          <t>OptionDebugLogging</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>bool</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>Enable verbose debug logging</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr"/>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>CategoryStatistics</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>10</v>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
           <t>OptionResetStats</t>
         </is>
       </c>
-      <c r="D56" t="inlineStr">
+      <c r="D57" t="inlineStr">
         <is>
           <t>bool</t>
         </is>
       </c>
-      <c r="E56" t="inlineStr">
+      <c r="E57" t="inlineStr">
         <is>
           <t>false</t>
         </is>
       </c>
-      <c r="F56" t="inlineStr">
+      <c r="F57" t="inlineStr">
         <is>
           <t>Toggle to reset all statistics</t>
         </is>
       </c>
-      <c r="G56" t="inlineStr"/>
+      <c r="G57" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Remove bleed from blunt damage, clean up VFX comments
- Removed BluntMultiplier ModOption and all related references
- Blunt damage already skipped in EventHooks.cs (no functional change)
- Updated IsDamageTypeAllowed to explicitly exclude blunt
- Cleaned up VFX comments to remove blunt-specific references
- All bleed DoTs now use same meshBone+renderer binding approach
- Updated build_presets_xlsx.py to reflect correct multiplier defaults
- Regenerated MENU_MOCK.xlsx (55 options, down from 56)
</commit_message>
<xml_diff>
--- a/MENU_MOCK.xlsx
+++ b/MENU_MOCK.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G57"/>
+  <dimension ref="A1:G56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -770,7 +770,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>OptionBluntMultiplier</t>
+          <t>OptionFireMultiplier</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -780,12 +780,12 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>0.5f</t>
+          <t>0.3f</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>DOT damage multiplier for blunt attacks. 0.0x disables DOT from blunt entirely.</t>
+          <t>DOT damage multiplier for fire attacks. While active, creature has Burning visual effect. 0.0x disables DOT from fire entirely.</t>
         </is>
       </c>
       <c r="G11" t="inlineStr"/>
@@ -801,7 +801,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>OptionFireMultiplier</t>
+          <t>OptionLightningMultiplier</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -811,12 +811,12 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>0.3f</t>
+          <t>1.5f</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>DOT damage multiplier for fire attacks. While active, creature has Burning visual effect. 0.0x disables DOT from fire entirely.</t>
+          <t>DOT damage multiplier for lightning attacks. While active, creature has Electrocute visual effect. 0.0x disables DOT from lightning entirely.</t>
         </is>
       </c>
       <c r="G12" t="inlineStr"/>
@@ -824,30 +824,30 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>CategoryDamageTypeMultipliers</t>
+          <t>CategoryZoneToggles</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>OptionLightningMultiplier</t>
+          <t>OptionThroatEnabled</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>float</t>
+          <t>bool</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>1.5f</t>
+          <t>true</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>DOT damage multiplier for lightning attacks. While active, creature has Electrocute visual effect. 0.0x disables DOT from lightning entirely.</t>
+          <t>Enable bleeding from throat wounds</t>
         </is>
       </c>
       <c r="G13" t="inlineStr"/>
@@ -859,11 +859,11 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>OptionThroatEnabled</t>
+          <t>OptionHeadEnabled</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -878,7 +878,7 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Enable bleeding from throat wounds</t>
+          <t>Enable bleeding from head wounds</t>
         </is>
       </c>
       <c r="G14" t="inlineStr"/>
@@ -890,11 +890,11 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>OptionHeadEnabled</t>
+          <t>OptionNeckEnabled</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -909,7 +909,7 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Enable bleeding from head wounds</t>
+          <t>Enable bleeding from neck wounds</t>
         </is>
       </c>
       <c r="G15" t="inlineStr"/>
@@ -921,11 +921,11 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>OptionNeckEnabled</t>
+          <t>OptionTorsoEnabled</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -940,7 +940,7 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Enable bleeding from neck wounds</t>
+          <t>Enable bleeding from torso wounds</t>
         </is>
       </c>
       <c r="G16" t="inlineStr"/>
@@ -952,11 +952,11 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>OptionTorsoEnabled</t>
+          <t>OptionArmEnabled</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -971,7 +971,7 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Enable bleeding from torso wounds</t>
+          <t>Enable bleeding from arm wounds</t>
         </is>
       </c>
       <c r="G17" t="inlineStr"/>
@@ -983,11 +983,11 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>OptionArmEnabled</t>
+          <t>OptionLegEnabled</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1002,7 +1002,7 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Enable bleeding from arm wounds</t>
+          <t>Enable bleeding from leg wounds</t>
         </is>
       </c>
       <c r="G18" t="inlineStr"/>
@@ -1014,11 +1014,11 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>OptionLegEnabled</t>
+          <t>OptionDismembermentEnabled</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -1033,7 +1033,7 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Enable bleeding from leg wounds</t>
+          <t>Enable bleeding from dismemberment</t>
         </is>
       </c>
       <c r="G19" t="inlineStr"/>
@@ -1041,30 +1041,30 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>CategoryZoneToggles</t>
+          <t>CategoryZoneThroat</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>OptionDismembermentEnabled</t>
+          <t>OptionThroatChance</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>bool</t>
+          <t>float</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>true</t>
+          <t>60f</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Enable bleeding from dismemberment</t>
+          <t>Chance for throat wounds to cause bleeding</t>
         </is>
       </c>
       <c r="G20" t="inlineStr"/>
@@ -1076,11 +1076,11 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>OptionThroatChance</t>
+          <t>OptionThroatDamage</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1090,12 +1090,12 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>60f</t>
+          <t>2.5f</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Chance for throat wounds to cause bleeding</t>
+          <t>Base damage per tick for throat wounds</t>
         </is>
       </c>
       <c r="G21" t="inlineStr"/>
@@ -1107,11 +1107,11 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>OptionThroatDamage</t>
+          <t>OptionThroatDuration</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -1121,12 +1121,12 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>2.5f</t>
+          <t>6.0f</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Base damage per tick for throat wounds</t>
+          <t>How long throat bleeds last</t>
         </is>
       </c>
       <c r="G22" t="inlineStr"/>
@@ -1138,11 +1138,11 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>OptionThroatDuration</t>
+          <t>OptionThroatFrequency</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -1152,12 +1152,12 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>6.0f</t>
+          <t>0.5f</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>How long throat bleeds last</t>
+          <t>Time between bleed ticks for throat wounds</t>
         </is>
       </c>
       <c r="G23" t="inlineStr"/>
@@ -1169,26 +1169,26 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>OptionThroatFrequency</t>
+          <t>OptionThroatStackLimit</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>float</t>
+          <t>int</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>0.5f</t>
+          <t>3</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Time between bleed ticks for throat wounds</t>
+          <t>Max stacks for throat wounds</t>
         </is>
       </c>
       <c r="G24" t="inlineStr"/>
@@ -1196,30 +1196,30 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>CategoryZoneThroat</t>
+          <t>CategoryZoneHead</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>OptionThroatStackLimit</t>
+          <t>OptionHeadChance</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>int</t>
+          <t>float</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>40f</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Max stacks for throat wounds</t>
+          <t>Chance for head wounds to cause bleeding</t>
         </is>
       </c>
       <c r="G25" t="inlineStr"/>
@@ -1231,11 +1231,11 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>OptionHeadChance</t>
+          <t>OptionHeadDamage</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1245,12 +1245,12 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>40f</t>
+          <t>1.5f</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Chance for head wounds to cause bleeding</t>
+          <t>Base damage per tick for head wounds</t>
         </is>
       </c>
       <c r="G26" t="inlineStr"/>
@@ -1262,11 +1262,11 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>OptionHeadDamage</t>
+          <t>OptionHeadDuration</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1276,12 +1276,12 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>1.5f</t>
+          <t>5.0f</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Base damage per tick for head wounds</t>
+          <t>How long head bleeds last</t>
         </is>
       </c>
       <c r="G27" t="inlineStr"/>
@@ -1293,11 +1293,11 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>OptionHeadDuration</t>
+          <t>OptionHeadFrequency</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1307,12 +1307,12 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>5.0f</t>
+          <t>0.5f</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>How long head bleeds last</t>
+          <t>Time between bleed ticks for head wounds</t>
         </is>
       </c>
       <c r="G28" t="inlineStr"/>
@@ -1324,26 +1324,26 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>OptionHeadFrequency</t>
+          <t>OptionHeadStackLimit</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>float</t>
+          <t>int</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>0.5f</t>
+          <t>3</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Time between bleed ticks for head wounds</t>
+          <t>Max stacks for head wounds</t>
         </is>
       </c>
       <c r="G29" t="inlineStr"/>
@@ -1351,30 +1351,30 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>CategoryZoneHead</t>
+          <t>CategoryZoneNeck</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>OptionHeadStackLimit</t>
+          <t>OptionNeckChance</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>int</t>
+          <t>float</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>55f</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Max stacks for head wounds</t>
+          <t>Chance for neck wounds to cause bleeding</t>
         </is>
       </c>
       <c r="G30" t="inlineStr"/>
@@ -1386,11 +1386,11 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>OptionNeckChance</t>
+          <t>OptionNeckDamage</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1400,12 +1400,12 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>55f</t>
+          <t>2.0f</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>Chance for neck wounds to cause bleeding</t>
+          <t>Base damage per tick for neck wounds</t>
         </is>
       </c>
       <c r="G31" t="inlineStr"/>
@@ -1417,11 +1417,11 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>OptionNeckDamage</t>
+          <t>OptionNeckDuration</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1431,12 +1431,12 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>2.0f</t>
+          <t>5.5f</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>Base damage per tick for neck wounds</t>
+          <t>How long neck bleeds last</t>
         </is>
       </c>
       <c r="G32" t="inlineStr"/>
@@ -1448,11 +1448,11 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>OptionNeckDuration</t>
+          <t>OptionNeckFrequency</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -1462,12 +1462,12 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>5.5f</t>
+          <t>0.5f</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>How long neck bleeds last</t>
+          <t>Time between bleed ticks for neck wounds</t>
         </is>
       </c>
       <c r="G33" t="inlineStr"/>
@@ -1479,26 +1479,26 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>OptionNeckFrequency</t>
+          <t>OptionNeckStackLimit</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>float</t>
+          <t>int</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>0.5f</t>
+          <t>3</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Time between bleed ticks for neck wounds</t>
+          <t>Max stacks for neck wounds</t>
         </is>
       </c>
       <c r="G34" t="inlineStr"/>
@@ -1506,30 +1506,30 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>CategoryZoneNeck</t>
+          <t>CategoryZoneTorso</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>OptionNeckStackLimit</t>
+          <t>OptionTorsoChance</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>int</t>
+          <t>float</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>35f</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>Max stacks for neck wounds</t>
+          <t>Chance for torso wounds to cause bleeding</t>
         </is>
       </c>
       <c r="G35" t="inlineStr"/>
@@ -1541,11 +1541,11 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>OptionTorsoChance</t>
+          <t>OptionTorsoDamage</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -1555,12 +1555,12 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>35f</t>
+          <t>1.0f</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>Chance for torso wounds to cause bleeding</t>
+          <t>Base damage per tick for torso wounds</t>
         </is>
       </c>
       <c r="G36" t="inlineStr"/>
@@ -1572,11 +1572,11 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>OptionTorsoDamage</t>
+          <t>OptionTorsoDuration</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -1586,12 +1586,12 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>1.0f</t>
+          <t>4.0f</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>Base damage per tick for torso wounds</t>
+          <t>How long torso bleeds last</t>
         </is>
       </c>
       <c r="G37" t="inlineStr"/>
@@ -1603,11 +1603,11 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>OptionTorsoDuration</t>
+          <t>OptionTorsoFrequency</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -1617,12 +1617,12 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>4.0f</t>
+          <t>0.5f</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>How long torso bleeds last</t>
+          <t>Time between bleed ticks for torso wounds</t>
         </is>
       </c>
       <c r="G38" t="inlineStr"/>
@@ -1634,26 +1634,26 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>OptionTorsoFrequency</t>
+          <t>OptionTorsoStackLimit</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>float</t>
+          <t>int</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>0.5f</t>
+          <t>5</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>Time between bleed ticks for torso wounds</t>
+          <t>Max stacks for torso wounds</t>
         </is>
       </c>
       <c r="G39" t="inlineStr"/>
@@ -1661,30 +1661,30 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>CategoryZoneTorso</t>
+          <t>CategoryZoneArm</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>OptionTorsoStackLimit</t>
+          <t>OptionArmChance</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>int</t>
+          <t>float</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>25f</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>Max stacks for torso wounds</t>
+          <t>Chance for arm wounds to cause bleeding</t>
         </is>
       </c>
       <c r="G40" t="inlineStr"/>
@@ -1696,11 +1696,11 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>OptionArmChance</t>
+          <t>OptionArmDamage</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -1710,12 +1710,12 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>25f</t>
+          <t>0.5f</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>Chance for arm wounds to cause bleeding</t>
+          <t>Base damage per tick for arm wounds</t>
         </is>
       </c>
       <c r="G41" t="inlineStr"/>
@@ -1727,11 +1727,11 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>OptionArmDamage</t>
+          <t>OptionArmDuration</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -1741,12 +1741,12 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>0.5f</t>
+          <t>3.0f</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>Base damage per tick for arm wounds</t>
+          <t>How long arm bleeds last</t>
         </is>
       </c>
       <c r="G42" t="inlineStr"/>
@@ -1758,11 +1758,11 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>OptionArmDuration</t>
+          <t>OptionArmFrequency</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -1772,12 +1772,12 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>3.0f</t>
+          <t>0.5f</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>How long arm bleeds last</t>
+          <t>Time between bleed ticks for arm wounds</t>
         </is>
       </c>
       <c r="G43" t="inlineStr"/>
@@ -1789,26 +1789,26 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>OptionArmFrequency</t>
+          <t>OptionArmStackLimit</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>float</t>
+          <t>int</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>0.5f</t>
+          <t>4</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>Time between bleed ticks for arm wounds</t>
+          <t>Max stacks for arm wounds</t>
         </is>
       </c>
       <c r="G44" t="inlineStr"/>
@@ -1816,30 +1816,30 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>CategoryZoneArm</t>
+          <t>CategoryZoneLeg</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>OptionArmStackLimit</t>
+          <t>OptionLegChance</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>int</t>
+          <t>float</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>30f</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>Max stacks for arm wounds</t>
+          <t>Chance for leg wounds to cause bleeding</t>
         </is>
       </c>
       <c r="G45" t="inlineStr"/>
@@ -1851,11 +1851,11 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>OptionLegChance</t>
+          <t>OptionLegDamage</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -1865,12 +1865,12 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>30f</t>
+          <t>0.75f</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>Chance for leg wounds to cause bleeding</t>
+          <t>Base damage per tick for leg wounds</t>
         </is>
       </c>
       <c r="G46" t="inlineStr"/>
@@ -1882,11 +1882,11 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>OptionLegDamage</t>
+          <t>OptionLegDuration</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -1896,12 +1896,12 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>0.75f</t>
+          <t>3.5f</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>Base damage per tick for leg wounds</t>
+          <t>How long leg bleeds last</t>
         </is>
       </c>
       <c r="G47" t="inlineStr"/>
@@ -1913,11 +1913,11 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>OptionLegDuration</t>
+          <t>OptionLegFrequency</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -1927,12 +1927,12 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>3.5f</t>
+          <t>0.5f</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>How long leg bleeds last</t>
+          <t>Time between bleed ticks for leg wounds</t>
         </is>
       </c>
       <c r="G48" t="inlineStr"/>
@@ -1944,26 +1944,26 @@
         </is>
       </c>
       <c r="B49" t="n">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>OptionLegFrequency</t>
+          <t>OptionLegStackLimit</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>float</t>
+          <t>int</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>0.5f</t>
+          <t>4</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>Time between bleed ticks for leg wounds</t>
+          <t>Max stacks for leg wounds</t>
         </is>
       </c>
       <c r="G49" t="inlineStr"/>
@@ -1971,30 +1971,30 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>CategoryZoneLeg</t>
+          <t>CategoryZoneDismemberment</t>
         </is>
       </c>
       <c r="B50" t="n">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>OptionLegStackLimit</t>
+          <t>OptionDismembermentChance</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>int</t>
+          <t>float</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>80f</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>Max stacks for leg wounds</t>
+          <t>Chance for dismemberment to cause bleeding</t>
         </is>
       </c>
       <c r="G50" t="inlineStr"/>
@@ -2006,11 +2006,11 @@
         </is>
       </c>
       <c r="B51" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>OptionDismembermentChance</t>
+          <t>OptionDismembermentDamage</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
@@ -2020,12 +2020,12 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>80f</t>
+          <t>3.0f</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>Chance for dismemberment to cause bleeding</t>
+          <t>Base damage per tick for dismemberment</t>
         </is>
       </c>
       <c r="G51" t="inlineStr"/>
@@ -2037,11 +2037,11 @@
         </is>
       </c>
       <c r="B52" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>OptionDismembermentDamage</t>
+          <t>OptionDismembermentDuration</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -2051,12 +2051,12 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>3.0f</t>
+          <t>8.0f</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>Base damage per tick for dismemberment</t>
+          <t>How long dismemberment bleeds last</t>
         </is>
       </c>
       <c r="G52" t="inlineStr"/>
@@ -2068,11 +2068,11 @@
         </is>
       </c>
       <c r="B53" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>OptionDismembermentDuration</t>
+          <t>OptionDismembermentFrequency</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -2082,12 +2082,12 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>8.0f</t>
+          <t>0.5f</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>How long dismemberment bleeds last</t>
+          <t>Time between bleed ticks for dismemberment</t>
         </is>
       </c>
       <c r="G53" t="inlineStr"/>
@@ -2099,26 +2099,26 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>OptionDismembermentFrequency</t>
+          <t>OptionDismembermentStackLimit</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>float</t>
+          <t>int</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>0.5f</t>
+          <t>1</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>Time between bleed ticks for dismemberment</t>
+          <t>Max stacks for dismemberment (per limb)</t>
         </is>
       </c>
       <c r="G54" t="inlineStr"/>
@@ -2126,30 +2126,30 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>CategoryZoneDismemberment</t>
+          <t>CategoryAdvanced</t>
         </is>
       </c>
       <c r="B55" t="n">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>OptionDismembermentStackLimit</t>
+          <t>OptionDebugLogging</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>int</t>
+          <t>bool</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>false</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>Max stacks for dismemberment (per limb)</t>
+          <t>Enable verbose debug logging</t>
         </is>
       </c>
       <c r="G55" t="inlineStr"/>
@@ -2157,7 +2157,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>CategoryAdvanced</t>
+          <t>CategoryStatistics</t>
         </is>
       </c>
       <c r="B56" t="n">
@@ -2165,7 +2165,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>OptionDebugLogging</t>
+          <t>OptionResetStats</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -2180,41 +2180,10 @@
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>Enable verbose debug logging</t>
+          <t>Toggle to reset all statistics</t>
         </is>
       </c>
       <c r="G56" t="inlineStr"/>
-    </row>
-    <row r="57">
-      <c r="A57" t="inlineStr">
-        <is>
-          <t>CategoryStatistics</t>
-        </is>
-      </c>
-      <c r="B57" t="n">
-        <v>10</v>
-      </c>
-      <c r="C57" t="inlineStr">
-        <is>
-          <t>OptionResetStats</t>
-        </is>
-      </c>
-      <c r="D57" t="inlineStr">
-        <is>
-          <t>bool</t>
-        </is>
-      </c>
-      <c r="E57" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="F57" t="inlineStr">
-        <is>
-          <t>Toggle to reset all statistics</t>
-        </is>
-      </c>
-      <c r="G57" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Remove Statistics category and move Advanced to bottom
</commit_message>
<xml_diff>
--- a/MENU_MOCK.xlsx
+++ b/MENU_MOCK.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G56"/>
+  <dimension ref="A1:G55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2154,37 +2154,6 @@
       </c>
       <c r="G55" t="inlineStr"/>
     </row>
-    <row r="56">
-      <c r="A56" t="inlineStr">
-        <is>
-          <t>CategoryStatistics</t>
-        </is>
-      </c>
-      <c r="B56" t="n">
-        <v>10</v>
-      </c>
-      <c r="C56" t="inlineStr">
-        <is>
-          <t>OptionResetStats</t>
-        </is>
-      </c>
-      <c r="D56" t="inlineStr">
-        <is>
-          <t>bool</t>
-        </is>
-      </c>
-      <c r="E56" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="F56" t="inlineStr">
-        <is>
-          <t>Toggle to reset all statistics</t>
-        </is>
-      </c>
-      <c r="G56" t="inlineStr"/>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
feat(CDoT): add performance metrics and debug overlay
- Add PerformanceMetrics.cs: tracks tick processing and effect counts
- Add DebugOverlay.cs: console-based debug logging when option enabled
- Add DebugOverlay toggle to Advanced options category
- Integrate into CDoTModule: Initialize/Draw/Shutdown hooks
- Regenerate MENU_MOCK.xlsx with new option
</commit_message>
<xml_diff>
--- a/MENU_MOCK.xlsx
+++ b/MENU_MOCK.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G55"/>
+  <dimension ref="A1:G56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2154,6 +2154,37 @@
       </c>
       <c r="G55" t="inlineStr"/>
     </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>CategoryAdvanced</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
+        <v>20</v>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>OptionDebugOverlay</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>bool</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>Enable periodic debug overlay logging with performance stats</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>